<commit_message>
fas system rev v1
</commit_message>
<xml_diff>
--- a/@Functions/ntadateexport.xlsx
+++ b/@Functions/ntadateexport.xlsx
@@ -13,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'nca-nta 2020'!$A$57:$I$126</definedName>
   </definedNames>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="0"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Received</t>
   </si>
   <si>
-    <t>January 08, 2020</t>
-  </si>
-  <si>
     <t>NCA-BMB-D-20-0000507</t>
   </si>
   <si>
@@ -71,21 +68,6 @@
     <t>RLIP January</t>
   </si>
   <si>
-    <t>PS February</t>
-  </si>
-  <si>
-    <t>MOOE February</t>
-  </si>
-  <si>
-    <t>RLIP February</t>
-  </si>
-  <si>
-    <t>January 29, 2020</t>
-  </si>
-  <si>
-    <t>January 30, 2020</t>
-  </si>
-  <si>
     <t>2020-01-006</t>
   </si>
   <si>
@@ -95,10 +77,13 @@
     <t>Funding support for the implementation of programs and projects (For Taal Volcano Eruption)</t>
   </si>
   <si>
-    <t>January 31, 2020</t>
+    <t>PS February</t>
   </si>
   <si>
-    <t>February 04, 2020</t>
+    <t>MOOE February</t>
+  </si>
+  <si>
+    <t>RLIP February</t>
   </si>
   <si>
     <t>NCA-BMB-D-20-0001108</t>
@@ -111,9 +96,6 @@
   </si>
   <si>
     <t>Death Benefit Claim</t>
-  </si>
-  <si>
-    <t>February 05, 2020</t>
   </si>
   <si>
     <t>2020-02-012</t>
@@ -268,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="71">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -428,6 +410,9 @@
     <xf xfId="0" fontId="5" numFmtId="49" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="3" numFmtId="165" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
@@ -478,276 +463,6 @@
     </xf>
     <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="0" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="167" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="49" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="168" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,7 +768,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E283" sqref="E283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1071,29 +786,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" customHeight="1" ht="15.75" s="7" customFormat="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="61"/>
+      <c r="C1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="64" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1104,1769 +819,1589 @@
       <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="63"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="64"/>
     </row>
     <row r="3" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A3" s="70" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="71" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="72" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="76">
-        <v>15183000</v>
-      </c>
-      <c r="H3" s="77">
-        <v>0</v>
-      </c>
-      <c r="I3" s="78">
-        <v>15183000</v>
-      </c>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A4" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="80" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="81" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="82" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="84" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="85">
-        <v>1999000</v>
-      </c>
-      <c r="H4" s="86">
-        <v>0</v>
-      </c>
-      <c r="I4" s="87">
-        <v>1999000</v>
-      </c>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
     </row>
     <row r="5" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A5" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="89" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="90" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="91" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="92" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="93" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="94">
-        <v>1799000</v>
-      </c>
-      <c r="H5" s="95">
-        <v>0</v>
-      </c>
-      <c r="I5" s="96">
-        <v>1799000</v>
-      </c>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
     </row>
     <row r="6" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A6" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="99" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="100" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="102" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="103">
-        <v>15183000</v>
-      </c>
-      <c r="H6" s="104">
-        <v>0</v>
-      </c>
-      <c r="I6" s="105">
-        <v>15183000</v>
-      </c>
+      <c r="A6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
     </row>
     <row r="7" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A7" s="106" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="107" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="108" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="109" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="110" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="111" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="112">
-        <v>1999000</v>
-      </c>
-      <c r="H7" s="113">
-        <v>0</v>
-      </c>
-      <c r="I7" s="114">
-        <v>1999000</v>
-      </c>
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
     </row>
     <row r="8" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A8" s="115" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="116" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="118" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="119" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="120" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="121">
-        <v>1798000</v>
-      </c>
-      <c r="H8" s="122">
-        <v>0</v>
-      </c>
-      <c r="I8" s="123">
-        <v>1798000</v>
-      </c>
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A9" s="124" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="125" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="126" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="127" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="128" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="129" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="130">
-        <v>500000</v>
-      </c>
-      <c r="H9" s="131">
-        <v>0</v>
-      </c>
-      <c r="I9" s="132">
-        <v>500000</v>
-      </c>
+      <c r="A9" s="53"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
     </row>
     <row r="10" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A10" s="133" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="134" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="135" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="136" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="137" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="138" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="139">
-        <v>296000</v>
-      </c>
-      <c r="H10" s="140">
-        <v>0</v>
-      </c>
-      <c r="I10" s="141">
-        <v>296000</v>
-      </c>
+      <c r="A10" s="53"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
     </row>
     <row r="11" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A11" s="142" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="143" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="144" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="145" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="146" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="147" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="148">
-        <v>688000</v>
-      </c>
-      <c r="H11" s="149">
-        <v>0</v>
-      </c>
-      <c r="I11" s="150">
-        <v>688000</v>
-      </c>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
     </row>
     <row r="12" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A12" s="151" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="152" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="153" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="154" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="155" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="156" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="157">
-        <v>100376</v>
-      </c>
-      <c r="H12" s="158">
-        <v>0</v>
-      </c>
-      <c r="I12" s="159">
-        <v>100376</v>
-      </c>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
     </row>
     <row r="13" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A13" s="53"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="49"/>
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
       <c r="F13" s="35"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
     </row>
     <row r="14" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="49"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
       <c r="F14" s="35"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
     </row>
     <row r="15" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A15" s="53"/>
-      <c r="B15" s="53"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="49"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
       <c r="F15" s="35"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A16" s="53"/>
-      <c r="B16" s="53"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="49"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
     </row>
     <row r="17" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
       <c r="C17" s="49"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
       <c r="F17" s="35"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
     </row>
     <row r="18" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
       <c r="C18" s="49"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
       <c r="F18" s="35"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
     </row>
     <row r="19" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="49"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
       <c r="F19" s="35"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
     </row>
     <row r="20" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="49"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
       <c r="F20" s="35"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
     </row>
     <row r="21" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A21" s="53"/>
-      <c r="B21" s="53"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="49"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
       <c r="F21" s="35"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
     </row>
     <row r="22" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="54"/>
       <c r="C22" s="49"/>
       <c r="D22" s="48"/>
       <c r="E22" s="48"/>
       <c r="F22" s="35"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
     </row>
     <row r="23" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A23" s="53"/>
-      <c r="B23" s="53"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
       <c r="C23" s="49"/>
       <c r="D23" s="48"/>
       <c r="E23" s="48"/>
       <c r="F23" s="35"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
     </row>
     <row r="24" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A24" s="53"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="49"/>
       <c r="D24" s="48"/>
       <c r="E24" s="48"/>
       <c r="F24" s="35"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
     </row>
     <row r="25" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A25" s="53"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="49"/>
       <c r="D25" s="48"/>
       <c r="E25" s="48"/>
       <c r="F25" s="35"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
     </row>
     <row r="26" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A26" s="53"/>
-      <c r="B26" s="53"/>
+      <c r="A26" s="54"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="49"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
     </row>
     <row r="27" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A27" s="53"/>
-      <c r="B27" s="53"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="49"/>
       <c r="D27" s="48"/>
       <c r="E27" s="48"/>
       <c r="F27" s="35"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="64"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
     </row>
     <row r="28" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A28" s="53"/>
-      <c r="B28" s="53"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="49"/>
       <c r="D28" s="48"/>
       <c r="E28" s="48"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
     </row>
     <row r="29" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A29" s="53"/>
-      <c r="B29" s="53"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="49"/>
       <c r="D29" s="48"/>
       <c r="E29" s="48"/>
       <c r="F29" s="35"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="65"/>
     </row>
     <row r="30" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A30" s="53"/>
-      <c r="B30" s="53"/>
+      <c r="A30" s="54"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="49"/>
       <c r="D30" s="48"/>
       <c r="E30" s="48"/>
       <c r="F30" s="35"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
     </row>
     <row r="31" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A31" s="53"/>
-      <c r="B31" s="53"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="49"/>
       <c r="D31" s="48"/>
       <c r="E31" s="48"/>
       <c r="F31" s="35"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
     </row>
     <row r="32" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A32" s="53"/>
-      <c r="B32" s="53"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="49"/>
       <c r="D32" s="48"/>
       <c r="E32" s="48"/>
       <c r="F32" s="35"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
     </row>
     <row r="33" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A33" s="53"/>
-      <c r="B33" s="53"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="54"/>
       <c r="C33" s="49"/>
       <c r="D33" s="48"/>
       <c r="E33" s="48"/>
       <c r="F33" s="35"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
     </row>
     <row r="34" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A34" s="53"/>
-      <c r="B34" s="53"/>
+      <c r="A34" s="54"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="49"/>
       <c r="D34" s="48"/>
       <c r="E34" s="48"/>
       <c r="F34" s="35"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
     </row>
     <row r="35" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A35" s="53"/>
-      <c r="B35" s="53"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="49"/>
       <c r="D35" s="48"/>
       <c r="E35" s="48"/>
       <c r="F35" s="35"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-      <c r="I35" s="64"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
     </row>
     <row r="36" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A36" s="53"/>
-      <c r="B36" s="53"/>
+      <c r="A36" s="54"/>
+      <c r="B36" s="54"/>
       <c r="C36" s="49"/>
       <c r="D36" s="48"/>
       <c r="E36" s="48"/>
       <c r="F36" s="35"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
     </row>
     <row r="37" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A37" s="53"/>
-      <c r="B37" s="53"/>
+      <c r="A37" s="54"/>
+      <c r="B37" s="54"/>
       <c r="C37" s="49"/>
       <c r="D37" s="48"/>
       <c r="E37" s="48"/>
       <c r="F37" s="35"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
     </row>
     <row r="38" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A38" s="53"/>
-      <c r="B38" s="53"/>
+      <c r="A38" s="54"/>
+      <c r="B38" s="54"/>
       <c r="C38" s="49"/>
       <c r="D38" s="48"/>
       <c r="E38" s="48"/>
       <c r="F38" s="35"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
     </row>
     <row r="39" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A39" s="53"/>
-      <c r="B39" s="53"/>
+      <c r="A39" s="54"/>
+      <c r="B39" s="54"/>
       <c r="C39" s="49"/>
       <c r="D39" s="48"/>
       <c r="E39" s="48"/>
       <c r="F39" s="35"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="64"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
     </row>
     <row r="40" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A40" s="53"/>
-      <c r="B40" s="53"/>
+      <c r="A40" s="54"/>
+      <c r="B40" s="54"/>
       <c r="C40" s="49"/>
       <c r="D40" s="48"/>
       <c r="E40" s="48"/>
       <c r="F40" s="35"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
     </row>
     <row r="41" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A41" s="53"/>
-      <c r="B41" s="53"/>
+      <c r="A41" s="54"/>
+      <c r="B41" s="54"/>
       <c r="C41" s="49"/>
       <c r="D41" s="48"/>
       <c r="E41" s="48"/>
       <c r="F41" s="35"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="64"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="65"/>
     </row>
     <row r="42" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A42" s="53"/>
-      <c r="B42" s="53"/>
+      <c r="A42" s="54"/>
+      <c r="B42" s="54"/>
       <c r="C42" s="49"/>
       <c r="D42" s="48"/>
       <c r="E42" s="48"/>
       <c r="F42" s="35"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="64"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="65"/>
     </row>
     <row r="43" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A43" s="53"/>
-      <c r="B43" s="53"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="49"/>
       <c r="D43" s="48"/>
       <c r="E43" s="48"/>
       <c r="F43" s="35"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="64"/>
-      <c r="I43" s="64"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="65"/>
     </row>
     <row r="44" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="54"/>
       <c r="C44" s="49"/>
       <c r="D44" s="48"/>
       <c r="E44" s="48"/>
       <c r="F44" s="35"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
     </row>
     <row r="45" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="54"/>
+      <c r="B45" s="54"/>
       <c r="C45" s="49"/>
       <c r="D45" s="48"/>
       <c r="E45" s="48"/>
       <c r="F45" s="35"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="65"/>
     </row>
     <row r="46" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A46" s="53"/>
-      <c r="B46" s="53"/>
+      <c r="A46" s="54"/>
+      <c r="B46" s="54"/>
       <c r="C46" s="49"/>
       <c r="D46" s="48"/>
       <c r="E46" s="48"/>
       <c r="F46" s="35"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="65"/>
     </row>
     <row r="47" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A47" s="53"/>
-      <c r="B47" s="53"/>
+      <c r="A47" s="54"/>
+      <c r="B47" s="54"/>
       <c r="C47" s="49"/>
       <c r="D47" s="48"/>
       <c r="E47" s="48"/>
       <c r="F47" s="35"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="64"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="65"/>
+      <c r="I47" s="65"/>
     </row>
     <row r="48" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A48" s="53"/>
-      <c r="B48" s="53"/>
+      <c r="A48" s="54"/>
+      <c r="B48" s="54"/>
       <c r="C48" s="49"/>
       <c r="D48" s="48"/>
       <c r="E48" s="48"/>
       <c r="F48" s="35"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="64"/>
+      <c r="G48" s="65"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="65"/>
     </row>
     <row r="49" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A49" s="53"/>
-      <c r="B49" s="53"/>
+      <c r="A49" s="54"/>
+      <c r="B49" s="54"/>
       <c r="C49" s="49"/>
       <c r="D49" s="48"/>
       <c r="E49" s="48"/>
       <c r="F49" s="35"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="64"/>
+      <c r="G49" s="65"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="65"/>
     </row>
     <row r="50" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A50" s="53"/>
-      <c r="B50" s="53"/>
+      <c r="A50" s="54"/>
+      <c r="B50" s="54"/>
       <c r="C50" s="49"/>
       <c r="D50" s="48"/>
       <c r="E50" s="48"/>
       <c r="F50" s="35"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="64"/>
+      <c r="G50" s="65"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="65"/>
     </row>
     <row r="51" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A51" s="53"/>
-      <c r="B51" s="53"/>
+      <c r="A51" s="54"/>
+      <c r="B51" s="54"/>
       <c r="C51" s="49"/>
       <c r="D51" s="48"/>
       <c r="E51" s="48"/>
       <c r="F51" s="35"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="64"/>
+      <c r="G51" s="65"/>
+      <c r="H51" s="65"/>
+      <c r="I51" s="65"/>
     </row>
     <row r="52" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A52" s="53"/>
-      <c r="B52" s="53"/>
+      <c r="A52" s="54"/>
+      <c r="B52" s="54"/>
       <c r="C52" s="49"/>
       <c r="D52" s="48"/>
       <c r="E52" s="48"/>
       <c r="F52" s="35"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="64"/>
+      <c r="G52" s="65"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="65"/>
     </row>
     <row r="53" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A53" s="53"/>
-      <c r="B53" s="53"/>
+      <c r="A53" s="54"/>
+      <c r="B53" s="54"/>
       <c r="C53" s="35"/>
       <c r="D53" s="48"/>
       <c r="E53" s="48"/>
       <c r="F53" s="35"/>
-      <c r="G53" s="65"/>
-      <c r="H53" s="65"/>
-      <c r="I53" s="64"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="65"/>
     </row>
     <row r="54" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A54" s="53"/>
-      <c r="B54" s="53"/>
+      <c r="A54" s="54"/>
+      <c r="B54" s="54"/>
       <c r="C54" s="35"/>
       <c r="D54" s="48"/>
       <c r="E54" s="48"/>
       <c r="F54" s="35"/>
-      <c r="G54" s="64"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="64"/>
+      <c r="G54" s="65"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="65"/>
     </row>
     <row r="55" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A55" s="53"/>
-      <c r="B55" s="53"/>
+      <c r="A55" s="54"/>
+      <c r="B55" s="54"/>
       <c r="C55" s="35"/>
       <c r="D55" s="48"/>
       <c r="E55" s="48"/>
       <c r="F55" s="35"/>
-      <c r="G55" s="64"/>
-      <c r="H55" s="64"/>
-      <c r="I55" s="64"/>
+      <c r="G55" s="65"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="65"/>
     </row>
     <row r="56" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A56" s="53"/>
-      <c r="B56" s="53"/>
+      <c r="A56" s="54"/>
+      <c r="B56" s="54"/>
       <c r="C56" s="35"/>
       <c r="D56" s="48"/>
       <c r="E56" s="48"/>
       <c r="F56" s="35"/>
-      <c r="G56" s="64"/>
-      <c r="H56" s="64"/>
-      <c r="I56" s="64"/>
+      <c r="G56" s="65"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="65"/>
     </row>
     <row r="57" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A57" s="53"/>
-      <c r="B57" s="53"/>
+      <c r="A57" s="54"/>
+      <c r="B57" s="54"/>
       <c r="C57" s="35"/>
       <c r="D57" s="48"/>
       <c r="E57" s="48"/>
       <c r="F57" s="35"/>
-      <c r="G57" s="64"/>
-      <c r="H57" s="64"/>
-      <c r="I57" s="64"/>
+      <c r="G57" s="65"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="65"/>
     </row>
     <row r="58" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A58" s="53"/>
-      <c r="B58" s="53"/>
+      <c r="A58" s="54"/>
+      <c r="B58" s="54"/>
       <c r="C58" s="35"/>
       <c r="D58" s="48"/>
       <c r="E58" s="48"/>
       <c r="F58" s="35"/>
-      <c r="G58" s="64"/>
-      <c r="H58" s="64"/>
-      <c r="I58" s="64"/>
+      <c r="G58" s="65"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="65"/>
     </row>
     <row r="59" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A59" s="53"/>
-      <c r="B59" s="53"/>
+      <c r="A59" s="54"/>
+      <c r="B59" s="54"/>
       <c r="C59" s="35"/>
       <c r="D59" s="48"/>
       <c r="E59" s="48"/>
       <c r="F59" s="35"/>
-      <c r="G59" s="64"/>
-      <c r="H59" s="64"/>
-      <c r="I59" s="64"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="65"/>
     </row>
     <row r="60" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A60" s="53"/>
-      <c r="B60" s="53"/>
+      <c r="A60" s="54"/>
+      <c r="B60" s="54"/>
       <c r="C60" s="35"/>
       <c r="D60" s="48"/>
       <c r="E60" s="48"/>
       <c r="F60" s="35"/>
-      <c r="G60" s="64"/>
-      <c r="H60" s="64"/>
-      <c r="I60" s="64"/>
+      <c r="G60" s="65"/>
+      <c r="H60" s="65"/>
+      <c r="I60" s="65"/>
     </row>
     <row r="61" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A61" s="53"/>
-      <c r="B61" s="53"/>
+      <c r="A61" s="54"/>
+      <c r="B61" s="54"/>
       <c r="C61" s="35"/>
       <c r="D61" s="48"/>
       <c r="E61" s="48"/>
       <c r="F61" s="35"/>
-      <c r="G61" s="64"/>
-      <c r="H61" s="64"/>
-      <c r="I61" s="64"/>
+      <c r="G61" s="65"/>
+      <c r="H61" s="65"/>
+      <c r="I61" s="65"/>
     </row>
     <row r="62" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A62" s="53"/>
-      <c r="B62" s="53"/>
+      <c r="A62" s="54"/>
+      <c r="B62" s="54"/>
       <c r="C62" s="35"/>
       <c r="D62" s="48"/>
       <c r="E62" s="48"/>
       <c r="F62" s="35"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="64"/>
-      <c r="I62" s="64"/>
+      <c r="G62" s="65"/>
+      <c r="H62" s="65"/>
+      <c r="I62" s="65"/>
     </row>
     <row r="63" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A63" s="53"/>
-      <c r="B63" s="53"/>
+      <c r="A63" s="54"/>
+      <c r="B63" s="54"/>
       <c r="C63" s="35"/>
       <c r="D63" s="48"/>
       <c r="E63" s="48"/>
       <c r="F63" s="35"/>
-      <c r="G63" s="64"/>
-      <c r="H63" s="64"/>
-      <c r="I63" s="64"/>
+      <c r="G63" s="65"/>
+      <c r="H63" s="65"/>
+      <c r="I63" s="65"/>
     </row>
     <row r="64" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A64" s="53"/>
-      <c r="B64" s="53"/>
+      <c r="A64" s="54"/>
+      <c r="B64" s="54"/>
       <c r="C64" s="35"/>
       <c r="D64" s="48"/>
       <c r="E64" s="48"/>
       <c r="F64" s="35"/>
-      <c r="G64" s="64"/>
-      <c r="H64" s="64"/>
-      <c r="I64" s="64"/>
+      <c r="G64" s="65"/>
+      <c r="H64" s="65"/>
+      <c r="I64" s="65"/>
     </row>
     <row r="65" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A65" s="53"/>
-      <c r="B65" s="53"/>
+      <c r="A65" s="54"/>
+      <c r="B65" s="54"/>
       <c r="C65" s="35"/>
       <c r="D65" s="48"/>
       <c r="E65" s="48"/>
       <c r="F65" s="35"/>
-      <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
-      <c r="I65" s="64"/>
+      <c r="G65" s="65"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="65"/>
     </row>
     <row r="66" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
       <c r="A66" s="35"/>
-      <c r="B66" s="53"/>
+      <c r="B66" s="54"/>
       <c r="C66" s="35"/>
       <c r="D66" s="48"/>
       <c r="E66" s="48"/>
       <c r="F66" s="35"/>
-      <c r="G66" s="64"/>
-      <c r="H66" s="64"/>
-      <c r="I66" s="64"/>
+      <c r="G66" s="65"/>
+      <c r="H66" s="65"/>
+      <c r="I66" s="65"/>
     </row>
     <row r="67" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
       <c r="A67" s="50"/>
-      <c r="B67" s="53"/>
+      <c r="B67" s="54"/>
       <c r="C67" s="35"/>
       <c r="D67" s="48"/>
       <c r="E67" s="48"/>
       <c r="F67" s="35"/>
-      <c r="G67" s="64"/>
-      <c r="H67" s="64"/>
-      <c r="I67" s="64"/>
+      <c r="G67" s="65"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="65"/>
     </row>
     <row r="68" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A68" s="53"/>
-      <c r="B68" s="53"/>
+      <c r="A68" s="54"/>
+      <c r="B68" s="54"/>
       <c r="C68" s="35"/>
       <c r="D68" s="48"/>
       <c r="E68" s="48"/>
       <c r="F68" s="35"/>
-      <c r="G68" s="64"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="64"/>
+      <c r="G68" s="65"/>
+      <c r="H68" s="65"/>
+      <c r="I68" s="65"/>
     </row>
     <row r="69" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A69" s="53"/>
-      <c r="B69" s="53"/>
+      <c r="A69" s="54"/>
+      <c r="B69" s="54"/>
       <c r="C69" s="49"/>
       <c r="D69" s="48"/>
       <c r="E69" s="48"/>
       <c r="F69" s="35"/>
-      <c r="G69" s="64"/>
-      <c r="H69" s="64"/>
-      <c r="I69" s="64"/>
+      <c r="G69" s="65"/>
+      <c r="H69" s="65"/>
+      <c r="I69" s="65"/>
     </row>
     <row r="70" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A70" s="53"/>
-      <c r="B70" s="53"/>
+      <c r="A70" s="54"/>
+      <c r="B70" s="54"/>
       <c r="C70" s="35"/>
       <c r="D70" s="48"/>
       <c r="E70" s="48"/>
       <c r="F70" s="35"/>
-      <c r="G70" s="64"/>
-      <c r="H70" s="64"/>
-      <c r="I70" s="64"/>
+      <c r="G70" s="65"/>
+      <c r="H70" s="65"/>
+      <c r="I70" s="65"/>
     </row>
     <row r="71" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A71" s="53"/>
-      <c r="B71" s="53"/>
+      <c r="A71" s="54"/>
+      <c r="B71" s="54"/>
       <c r="C71" s="35"/>
       <c r="D71" s="48"/>
       <c r="E71" s="48"/>
       <c r="F71" s="35"/>
-      <c r="G71" s="64"/>
-      <c r="H71" s="64"/>
-      <c r="I71" s="64"/>
+      <c r="G71" s="65"/>
+      <c r="H71" s="65"/>
+      <c r="I71" s="65"/>
     </row>
     <row r="72" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A72" s="53"/>
-      <c r="B72" s="53"/>
+      <c r="A72" s="54"/>
+      <c r="B72" s="54"/>
       <c r="C72" s="35"/>
       <c r="D72" s="48"/>
       <c r="E72" s="48"/>
       <c r="F72" s="35"/>
-      <c r="G72" s="64"/>
-      <c r="H72" s="64"/>
-      <c r="I72" s="64"/>
+      <c r="G72" s="65"/>
+      <c r="H72" s="65"/>
+      <c r="I72" s="65"/>
     </row>
     <row r="73" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A73" s="53"/>
-      <c r="B73" s="53"/>
+      <c r="A73" s="54"/>
+      <c r="B73" s="54"/>
       <c r="C73" s="35"/>
       <c r="D73" s="48"/>
       <c r="E73" s="48"/>
       <c r="F73" s="35"/>
-      <c r="G73" s="64"/>
-      <c r="H73" s="64"/>
-      <c r="I73" s="64"/>
+      <c r="G73" s="65"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="65"/>
     </row>
     <row r="74" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A74" s="53"/>
-      <c r="B74" s="53"/>
+      <c r="A74" s="54"/>
+      <c r="B74" s="54"/>
       <c r="C74" s="35"/>
       <c r="D74" s="47"/>
       <c r="E74" s="47"/>
       <c r="F74" s="47"/>
-      <c r="G74" s="64"/>
-      <c r="H74" s="64"/>
-      <c r="I74" s="64"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="65"/>
     </row>
     <row r="75" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A75" s="53"/>
-      <c r="B75" s="53"/>
+      <c r="A75" s="54"/>
+      <c r="B75" s="54"/>
       <c r="C75" s="35"/>
       <c r="D75" s="47"/>
       <c r="E75" s="47"/>
       <c r="F75" s="49"/>
-      <c r="G75" s="64"/>
-      <c r="H75" s="64"/>
-      <c r="I75" s="64"/>
+      <c r="G75" s="65"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="65"/>
     </row>
     <row r="76" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A76" s="53"/>
-      <c r="B76" s="53"/>
+      <c r="A76" s="54"/>
+      <c r="B76" s="54"/>
       <c r="C76" s="35"/>
       <c r="D76" s="48"/>
       <c r="E76" s="48"/>
       <c r="F76" s="35"/>
-      <c r="G76" s="64"/>
-      <c r="H76" s="64"/>
-      <c r="I76" s="64"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="65"/>
     </row>
     <row r="77" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A77" s="53"/>
-      <c r="B77" s="53"/>
+      <c r="A77" s="54"/>
+      <c r="B77" s="54"/>
       <c r="C77" s="35"/>
       <c r="D77" s="48"/>
       <c r="E77" s="48"/>
       <c r="F77" s="35"/>
-      <c r="G77" s="64"/>
-      <c r="H77" s="64"/>
-      <c r="I77" s="64"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="65"/>
     </row>
     <row r="78" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A78" s="53"/>
-      <c r="B78" s="53"/>
+      <c r="A78" s="54"/>
+      <c r="B78" s="54"/>
       <c r="C78" s="35"/>
       <c r="D78" s="48"/>
       <c r="E78" s="48"/>
       <c r="F78" s="35"/>
-      <c r="G78" s="64"/>
-      <c r="H78" s="64"/>
-      <c r="I78" s="64"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="65"/>
     </row>
     <row r="79" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A79" s="53"/>
-      <c r="B79" s="53"/>
+      <c r="A79" s="54"/>
+      <c r="B79" s="54"/>
       <c r="C79" s="35"/>
       <c r="D79" s="48"/>
       <c r="E79" s="48"/>
       <c r="F79" s="35"/>
-      <c r="G79" s="64"/>
-      <c r="H79" s="64"/>
-      <c r="I79" s="64"/>
+      <c r="G79" s="65"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="65"/>
     </row>
     <row r="80" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A80" s="53"/>
-      <c r="B80" s="53"/>
+      <c r="A80" s="54"/>
+      <c r="B80" s="54"/>
       <c r="C80" s="35"/>
       <c r="D80" s="48"/>
       <c r="E80" s="48"/>
       <c r="F80" s="35"/>
-      <c r="G80" s="64"/>
-      <c r="H80" s="64"/>
-      <c r="I80" s="64"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="65"/>
     </row>
     <row r="81" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A81" s="53"/>
-      <c r="B81" s="53"/>
+      <c r="A81" s="54"/>
+      <c r="B81" s="54"/>
       <c r="C81" s="35"/>
       <c r="D81" s="48"/>
       <c r="E81" s="48"/>
       <c r="F81" s="35"/>
-      <c r="G81" s="64"/>
-      <c r="H81" s="64"/>
-      <c r="I81" s="64"/>
+      <c r="G81" s="65"/>
+      <c r="H81" s="65"/>
+      <c r="I81" s="65"/>
     </row>
     <row r="82" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A82" s="53"/>
-      <c r="B82" s="53"/>
+      <c r="A82" s="54"/>
+      <c r="B82" s="54"/>
       <c r="C82" s="35"/>
       <c r="D82" s="48"/>
       <c r="E82" s="48"/>
       <c r="F82" s="35"/>
-      <c r="G82" s="64"/>
-      <c r="H82" s="64"/>
-      <c r="I82" s="64"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="65"/>
     </row>
     <row r="83" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A83" s="53"/>
-      <c r="B83" s="53"/>
+      <c r="A83" s="54"/>
+      <c r="B83" s="54"/>
       <c r="C83" s="35"/>
       <c r="D83" s="48"/>
       <c r="E83" s="48"/>
       <c r="F83" s="35"/>
-      <c r="G83" s="64"/>
-      <c r="H83" s="64"/>
-      <c r="I83" s="64"/>
+      <c r="G83" s="65"/>
+      <c r="H83" s="65"/>
+      <c r="I83" s="65"/>
     </row>
     <row r="84" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A84" s="53"/>
-      <c r="B84" s="53"/>
+      <c r="A84" s="54"/>
+      <c r="B84" s="54"/>
       <c r="C84" s="35"/>
       <c r="D84" s="48"/>
       <c r="E84" s="48"/>
       <c r="F84" s="35"/>
-      <c r="G84" s="64"/>
-      <c r="H84" s="64"/>
-      <c r="I84" s="64"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+      <c r="I84" s="65"/>
     </row>
     <row r="85" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A85" s="53"/>
-      <c r="B85" s="53"/>
+      <c r="A85" s="54"/>
+      <c r="B85" s="54"/>
       <c r="C85" s="35"/>
       <c r="D85" s="48"/>
       <c r="E85" s="48"/>
       <c r="F85" s="35"/>
-      <c r="G85" s="64"/>
-      <c r="H85" s="64"/>
-      <c r="I85" s="64"/>
+      <c r="G85" s="65"/>
+      <c r="H85" s="65"/>
+      <c r="I85" s="65"/>
     </row>
     <row r="86" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A86" s="53"/>
-      <c r="B86" s="53"/>
+      <c r="A86" s="54"/>
+      <c r="B86" s="54"/>
       <c r="C86" s="35"/>
       <c r="D86" s="48"/>
       <c r="E86" s="48"/>
       <c r="F86" s="35"/>
-      <c r="G86" s="64"/>
-      <c r="H86" s="64"/>
-      <c r="I86" s="64"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="65"/>
     </row>
     <row r="87" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A87" s="53"/>
-      <c r="B87" s="53"/>
+      <c r="A87" s="54"/>
+      <c r="B87" s="54"/>
       <c r="C87" s="35"/>
       <c r="D87" s="48"/>
       <c r="E87" s="48"/>
       <c r="F87" s="35"/>
-      <c r="G87" s="64"/>
-      <c r="H87" s="64"/>
-      <c r="I87" s="64"/>
+      <c r="G87" s="65"/>
+      <c r="H87" s="65"/>
+      <c r="I87" s="65"/>
     </row>
     <row r="88" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A88" s="53"/>
-      <c r="B88" s="53"/>
+      <c r="A88" s="54"/>
+      <c r="B88" s="54"/>
       <c r="C88" s="35"/>
       <c r="D88" s="48"/>
       <c r="E88" s="48"/>
       <c r="F88" s="35"/>
-      <c r="G88" s="64"/>
-      <c r="H88" s="64"/>
-      <c r="I88" s="64"/>
+      <c r="G88" s="65"/>
+      <c r="H88" s="65"/>
+      <c r="I88" s="65"/>
     </row>
     <row r="89" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A89" s="53"/>
-      <c r="B89" s="53"/>
+      <c r="A89" s="54"/>
+      <c r="B89" s="54"/>
       <c r="C89" s="35"/>
       <c r="D89" s="48"/>
       <c r="E89" s="48"/>
       <c r="F89" s="35"/>
-      <c r="G89" s="64"/>
-      <c r="H89" s="64"/>
-      <c r="I89" s="64"/>
+      <c r="G89" s="65"/>
+      <c r="H89" s="65"/>
+      <c r="I89" s="65"/>
     </row>
     <row r="90" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A90" s="53"/>
-      <c r="B90" s="53"/>
+      <c r="A90" s="54"/>
+      <c r="B90" s="54"/>
       <c r="C90" s="35"/>
       <c r="D90" s="48"/>
       <c r="E90" s="48"/>
       <c r="F90" s="35"/>
-      <c r="G90" s="64"/>
-      <c r="H90" s="64"/>
-      <c r="I90" s="64"/>
+      <c r="G90" s="65"/>
+      <c r="H90" s="65"/>
+      <c r="I90" s="65"/>
     </row>
     <row r="91" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A91" s="53"/>
-      <c r="B91" s="53"/>
+      <c r="A91" s="54"/>
+      <c r="B91" s="54"/>
       <c r="C91" s="35"/>
       <c r="D91" s="48"/>
       <c r="E91" s="48"/>
       <c r="F91" s="35"/>
-      <c r="G91" s="64"/>
-      <c r="H91" s="64"/>
-      <c r="I91" s="64"/>
+      <c r="G91" s="65"/>
+      <c r="H91" s="65"/>
+      <c r="I91" s="65"/>
     </row>
     <row r="92" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A92" s="53"/>
-      <c r="B92" s="53"/>
+      <c r="A92" s="54"/>
+      <c r="B92" s="54"/>
       <c r="C92" s="35"/>
       <c r="D92" s="48"/>
       <c r="E92" s="48"/>
       <c r="F92" s="35"/>
-      <c r="G92" s="64"/>
-      <c r="H92" s="64"/>
-      <c r="I92" s="64"/>
+      <c r="G92" s="65"/>
+      <c r="H92" s="65"/>
+      <c r="I92" s="65"/>
     </row>
     <row r="93" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A93" s="53"/>
-      <c r="B93" s="53"/>
+      <c r="A93" s="54"/>
+      <c r="B93" s="54"/>
       <c r="C93" s="35"/>
       <c r="D93" s="48"/>
       <c r="E93" s="48"/>
       <c r="F93" s="35"/>
-      <c r="G93" s="64"/>
-      <c r="H93" s="64"/>
-      <c r="I93" s="64"/>
+      <c r="G93" s="65"/>
+      <c r="H93" s="65"/>
+      <c r="I93" s="65"/>
     </row>
     <row r="94" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A94" s="53"/>
-      <c r="B94" s="53"/>
+      <c r="A94" s="54"/>
+      <c r="B94" s="54"/>
       <c r="C94" s="35"/>
       <c r="D94" s="48"/>
       <c r="E94" s="48"/>
       <c r="F94" s="35"/>
-      <c r="G94" s="64"/>
-      <c r="H94" s="64"/>
-      <c r="I94" s="64"/>
+      <c r="G94" s="65"/>
+      <c r="H94" s="65"/>
+      <c r="I94" s="65"/>
     </row>
     <row r="95" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A95" s="53"/>
-      <c r="B95" s="53"/>
+      <c r="A95" s="54"/>
+      <c r="B95" s="54"/>
       <c r="C95" s="35"/>
       <c r="D95" s="48"/>
       <c r="E95" s="48"/>
       <c r="F95" s="35"/>
-      <c r="G95" s="64"/>
-      <c r="H95" s="64"/>
-      <c r="I95" s="64"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
     </row>
     <row r="96" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A96" s="53"/>
-      <c r="B96" s="53"/>
+      <c r="A96" s="54"/>
+      <c r="B96" s="54"/>
       <c r="C96" s="35"/>
       <c r="D96" s="48"/>
       <c r="E96" s="48"/>
       <c r="F96" s="35"/>
-      <c r="G96" s="64"/>
-      <c r="H96" s="64"/>
-      <c r="I96" s="64"/>
+      <c r="G96" s="65"/>
+      <c r="H96" s="65"/>
+      <c r="I96" s="65"/>
     </row>
     <row r="97" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A97" s="53"/>
-      <c r="B97" s="53"/>
+      <c r="A97" s="54"/>
+      <c r="B97" s="54"/>
       <c r="C97" s="35"/>
       <c r="D97" s="48"/>
       <c r="E97" s="48"/>
       <c r="F97" s="35"/>
-      <c r="G97" s="64"/>
-      <c r="H97" s="64"/>
-      <c r="I97" s="64"/>
+      <c r="G97" s="65"/>
+      <c r="H97" s="65"/>
+      <c r="I97" s="65"/>
     </row>
     <row r="98" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A98" s="53"/>
-      <c r="B98" s="53"/>
+      <c r="A98" s="54"/>
+      <c r="B98" s="54"/>
       <c r="C98" s="35"/>
       <c r="D98" s="48"/>
       <c r="E98" s="48"/>
       <c r="F98" s="35"/>
-      <c r="G98" s="64"/>
-      <c r="H98" s="64"/>
-      <c r="I98" s="64"/>
+      <c r="G98" s="65"/>
+      <c r="H98" s="65"/>
+      <c r="I98" s="65"/>
     </row>
     <row r="99" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A99" s="53"/>
-      <c r="B99" s="53"/>
+      <c r="A99" s="54"/>
+      <c r="B99" s="54"/>
       <c r="C99" s="35"/>
       <c r="D99" s="48"/>
       <c r="E99" s="48"/>
       <c r="F99" s="35"/>
-      <c r="G99" s="64"/>
-      <c r="H99" s="64"/>
-      <c r="I99" s="64"/>
+      <c r="G99" s="65"/>
+      <c r="H99" s="65"/>
+      <c r="I99" s="65"/>
     </row>
     <row r="100" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A100" s="53"/>
-      <c r="B100" s="53"/>
+      <c r="A100" s="54"/>
+      <c r="B100" s="54"/>
       <c r="C100" s="35"/>
       <c r="D100" s="48"/>
       <c r="E100" s="48"/>
       <c r="F100" s="35"/>
-      <c r="G100" s="64"/>
-      <c r="H100" s="64"/>
-      <c r="I100" s="64"/>
+      <c r="G100" s="65"/>
+      <c r="H100" s="65"/>
+      <c r="I100" s="65"/>
     </row>
     <row r="101" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A101" s="53"/>
-      <c r="B101" s="53"/>
+      <c r="A101" s="54"/>
+      <c r="B101" s="54"/>
       <c r="C101" s="35"/>
       <c r="D101" s="48"/>
       <c r="E101" s="48"/>
       <c r="F101" s="35"/>
-      <c r="G101" s="64"/>
-      <c r="H101" s="64"/>
-      <c r="I101" s="64"/>
+      <c r="G101" s="65"/>
+      <c r="H101" s="65"/>
+      <c r="I101" s="65"/>
     </row>
     <row r="102" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A102" s="53"/>
-      <c r="B102" s="53"/>
+      <c r="A102" s="54"/>
+      <c r="B102" s="54"/>
       <c r="C102" s="35"/>
       <c r="D102" s="48"/>
       <c r="E102" s="48"/>
       <c r="F102" s="35"/>
-      <c r="G102" s="64"/>
-      <c r="H102" s="64"/>
-      <c r="I102" s="64"/>
+      <c r="G102" s="65"/>
+      <c r="H102" s="65"/>
+      <c r="I102" s="65"/>
     </row>
     <row r="103" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A103" s="53"/>
-      <c r="B103" s="53"/>
+      <c r="A103" s="54"/>
+      <c r="B103" s="54"/>
       <c r="C103" s="35"/>
       <c r="D103" s="48"/>
       <c r="E103" s="48"/>
       <c r="F103" s="35"/>
-      <c r="G103" s="64"/>
-      <c r="H103" s="64"/>
-      <c r="I103" s="64"/>
+      <c r="G103" s="65"/>
+      <c r="H103" s="65"/>
+      <c r="I103" s="65"/>
     </row>
     <row r="104" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A104" s="53"/>
-      <c r="B104" s="53"/>
+      <c r="A104" s="54"/>
+      <c r="B104" s="54"/>
       <c r="C104" s="35"/>
       <c r="D104" s="48"/>
       <c r="E104" s="48"/>
       <c r="F104" s="35"/>
-      <c r="G104" s="64"/>
-      <c r="H104" s="64"/>
-      <c r="I104" s="64"/>
+      <c r="G104" s="65"/>
+      <c r="H104" s="65"/>
+      <c r="I104" s="65"/>
     </row>
     <row r="105" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A105" s="53"/>
-      <c r="B105" s="53"/>
+      <c r="A105" s="54"/>
+      <c r="B105" s="54"/>
       <c r="C105" s="35"/>
       <c r="D105" s="48"/>
       <c r="E105" s="48"/>
       <c r="F105" s="35"/>
-      <c r="G105" s="64"/>
-      <c r="H105" s="64"/>
-      <c r="I105" s="64"/>
+      <c r="G105" s="65"/>
+      <c r="H105" s="65"/>
+      <c r="I105" s="65"/>
     </row>
     <row r="106" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A106" s="53"/>
-      <c r="B106" s="53"/>
+      <c r="A106" s="54"/>
+      <c r="B106" s="54"/>
       <c r="C106" s="35"/>
       <c r="D106" s="48"/>
       <c r="E106" s="48"/>
       <c r="F106" s="35"/>
-      <c r="G106" s="64"/>
-      <c r="H106" s="64"/>
-      <c r="I106" s="64"/>
+      <c r="G106" s="65"/>
+      <c r="H106" s="65"/>
+      <c r="I106" s="65"/>
     </row>
     <row r="107" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A107" s="53"/>
-      <c r="B107" s="53"/>
+      <c r="A107" s="54"/>
+      <c r="B107" s="54"/>
       <c r="C107" s="35"/>
       <c r="D107" s="48"/>
       <c r="E107" s="48"/>
       <c r="F107" s="35"/>
-      <c r="G107" s="64"/>
-      <c r="H107" s="64"/>
-      <c r="I107" s="64"/>
+      <c r="G107" s="65"/>
+      <c r="H107" s="65"/>
+      <c r="I107" s="65"/>
     </row>
     <row r="108" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A108" s="53"/>
-      <c r="B108" s="53"/>
+      <c r="A108" s="54"/>
+      <c r="B108" s="54"/>
       <c r="C108" s="35"/>
       <c r="D108" s="48"/>
       <c r="E108" s="48"/>
       <c r="F108" s="35"/>
-      <c r="G108" s="64"/>
-      <c r="H108" s="64"/>
-      <c r="I108" s="64"/>
+      <c r="G108" s="65"/>
+      <c r="H108" s="65"/>
+      <c r="I108" s="65"/>
     </row>
     <row r="109" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A109" s="53"/>
-      <c r="B109" s="53"/>
+      <c r="A109" s="54"/>
+      <c r="B109" s="54"/>
       <c r="C109" s="35"/>
       <c r="D109" s="48"/>
       <c r="E109" s="48"/>
       <c r="F109" s="35"/>
-      <c r="G109" s="64"/>
-      <c r="H109" s="64"/>
-      <c r="I109" s="64"/>
+      <c r="G109" s="65"/>
+      <c r="H109" s="65"/>
+      <c r="I109" s="65"/>
     </row>
     <row r="110" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A110" s="53"/>
-      <c r="B110" s="53"/>
+      <c r="A110" s="54"/>
+      <c r="B110" s="54"/>
       <c r="C110" s="35"/>
       <c r="D110" s="48"/>
       <c r="E110" s="48"/>
       <c r="F110" s="35"/>
-      <c r="G110" s="64"/>
-      <c r="H110" s="64"/>
-      <c r="I110" s="64"/>
+      <c r="G110" s="65"/>
+      <c r="H110" s="65"/>
+      <c r="I110" s="65"/>
     </row>
     <row r="111" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A111" s="53"/>
-      <c r="B111" s="53"/>
+      <c r="A111" s="54"/>
+      <c r="B111" s="54"/>
       <c r="C111" s="35"/>
       <c r="D111" s="48"/>
       <c r="E111" s="48"/>
       <c r="F111" s="35"/>
-      <c r="G111" s="64"/>
-      <c r="H111" s="64"/>
-      <c r="I111" s="64"/>
+      <c r="G111" s="65"/>
+      <c r="H111" s="65"/>
+      <c r="I111" s="65"/>
     </row>
     <row r="112" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A112" s="53"/>
-      <c r="B112" s="53"/>
+      <c r="A112" s="54"/>
+      <c r="B112" s="54"/>
       <c r="C112" s="35"/>
       <c r="D112" s="48"/>
       <c r="E112" s="48"/>
       <c r="F112" s="35"/>
-      <c r="G112" s="64"/>
-      <c r="H112" s="64"/>
-      <c r="I112" s="64"/>
+      <c r="G112" s="65"/>
+      <c r="H112" s="65"/>
+      <c r="I112" s="65"/>
     </row>
     <row r="113" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A113" s="53"/>
-      <c r="B113" s="53"/>
+      <c r="A113" s="54"/>
+      <c r="B113" s="54"/>
       <c r="C113" s="35"/>
       <c r="D113" s="48"/>
       <c r="E113" s="48"/>
       <c r="F113" s="35"/>
-      <c r="G113" s="64"/>
-      <c r="H113" s="64"/>
-      <c r="I113" s="64"/>
+      <c r="G113" s="65"/>
+      <c r="H113" s="65"/>
+      <c r="I113" s="65"/>
     </row>
     <row r="114" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A114" s="53"/>
-      <c r="B114" s="53"/>
+      <c r="A114" s="54"/>
+      <c r="B114" s="54"/>
       <c r="C114" s="35"/>
       <c r="D114" s="48"/>
       <c r="E114" s="48"/>
       <c r="F114" s="35"/>
-      <c r="G114" s="64"/>
-      <c r="H114" s="64"/>
-      <c r="I114" s="64"/>
+      <c r="G114" s="65"/>
+      <c r="H114" s="65"/>
+      <c r="I114" s="65"/>
     </row>
     <row r="115" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A115" s="53"/>
-      <c r="B115" s="53"/>
+      <c r="A115" s="54"/>
+      <c r="B115" s="54"/>
       <c r="C115" s="35"/>
       <c r="D115" s="48"/>
       <c r="E115" s="48"/>
       <c r="F115" s="35"/>
-      <c r="G115" s="64"/>
-      <c r="H115" s="64"/>
-      <c r="I115" s="64"/>
+      <c r="G115" s="65"/>
+      <c r="H115" s="65"/>
+      <c r="I115" s="65"/>
     </row>
     <row r="116" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A116" s="53"/>
-      <c r="B116" s="53"/>
+      <c r="A116" s="54"/>
+      <c r="B116" s="54"/>
       <c r="C116" s="35"/>
       <c r="D116" s="48"/>
       <c r="E116" s="48"/>
       <c r="F116" s="35"/>
-      <c r="G116" s="64"/>
-      <c r="H116" s="64"/>
-      <c r="I116" s="64"/>
+      <c r="G116" s="65"/>
+      <c r="H116" s="65"/>
+      <c r="I116" s="65"/>
     </row>
     <row r="117" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A117" s="53"/>
-      <c r="B117" s="53"/>
+      <c r="A117" s="54"/>
+      <c r="B117" s="54"/>
       <c r="C117" s="35"/>
       <c r="D117" s="48"/>
       <c r="E117" s="48"/>
       <c r="F117" s="35"/>
-      <c r="G117" s="64"/>
-      <c r="H117" s="64"/>
-      <c r="I117" s="64"/>
+      <c r="G117" s="65"/>
+      <c r="H117" s="65"/>
+      <c r="I117" s="65"/>
     </row>
     <row r="118" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A118" s="53"/>
-      <c r="B118" s="53"/>
+      <c r="A118" s="54"/>
+      <c r="B118" s="54"/>
       <c r="C118" s="35"/>
       <c r="D118" s="48"/>
       <c r="E118" s="48"/>
       <c r="F118" s="35"/>
-      <c r="G118" s="64"/>
-      <c r="H118" s="64"/>
-      <c r="I118" s="64"/>
+      <c r="G118" s="65"/>
+      <c r="H118" s="65"/>
+      <c r="I118" s="65"/>
     </row>
     <row r="119" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A119" s="53"/>
-      <c r="B119" s="53"/>
+      <c r="A119" s="54"/>
+      <c r="B119" s="54"/>
       <c r="C119" s="35"/>
       <c r="D119" s="48"/>
       <c r="E119" s="48"/>
       <c r="F119" s="35"/>
-      <c r="G119" s="64"/>
-      <c r="H119" s="64"/>
-      <c r="I119" s="64"/>
+      <c r="G119" s="65"/>
+      <c r="H119" s="65"/>
+      <c r="I119" s="65"/>
     </row>
     <row r="120" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A120" s="54"/>
-      <c r="B120" s="54"/>
+      <c r="A120" s="55"/>
+      <c r="B120" s="55"/>
       <c r="C120" s="51"/>
-      <c r="D120" s="55"/>
-      <c r="E120" s="55"/>
+      <c r="D120" s="56"/>
+      <c r="E120" s="56"/>
       <c r="F120" s="51"/>
-      <c r="G120" s="66"/>
-      <c r="H120" s="66"/>
-      <c r="I120" s="66"/>
+      <c r="G120" s="67"/>
+      <c r="H120" s="67"/>
+      <c r="I120" s="67"/>
     </row>
     <row r="121" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A121" s="54"/>
-      <c r="B121" s="54"/>
+      <c r="A121" s="55"/>
+      <c r="B121" s="55"/>
       <c r="C121" s="51"/>
-      <c r="D121" s="55"/>
-      <c r="E121" s="55"/>
+      <c r="D121" s="56"/>
+      <c r="E121" s="56"/>
       <c r="F121" s="51"/>
-      <c r="G121" s="66"/>
-      <c r="H121" s="66"/>
-      <c r="I121" s="66"/>
+      <c r="G121" s="67"/>
+      <c r="H121" s="67"/>
+      <c r="I121" s="67"/>
     </row>
     <row r="122" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A122" s="54"/>
-      <c r="B122" s="54"/>
+      <c r="A122" s="55"/>
+      <c r="B122" s="55"/>
       <c r="C122" s="51"/>
-      <c r="D122" s="55"/>
-      <c r="E122" s="55"/>
+      <c r="D122" s="56"/>
+      <c r="E122" s="56"/>
       <c r="F122" s="51"/>
-      <c r="G122" s="66"/>
-      <c r="H122" s="66"/>
-      <c r="I122" s="66"/>
+      <c r="G122" s="67"/>
+      <c r="H122" s="67"/>
+      <c r="I122" s="67"/>
     </row>
     <row r="123" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A123" s="53"/>
-      <c r="B123" s="53"/>
+      <c r="A123" s="54"/>
+      <c r="B123" s="54"/>
       <c r="C123" s="49"/>
       <c r="D123" s="48"/>
       <c r="E123" s="48"/>
       <c r="F123" s="35"/>
-      <c r="G123" s="64"/>
-      <c r="H123" s="64"/>
-      <c r="I123" s="64"/>
+      <c r="G123" s="65"/>
+      <c r="H123" s="65"/>
+      <c r="I123" s="65"/>
     </row>
     <row r="124" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A124" s="53"/>
-      <c r="B124" s="53"/>
+      <c r="A124" s="54"/>
+      <c r="B124" s="54"/>
       <c r="C124" s="49"/>
       <c r="D124" s="48"/>
       <c r="E124" s="48"/>
       <c r="F124" s="35"/>
-      <c r="G124" s="64"/>
-      <c r="H124" s="64"/>
-      <c r="I124" s="64"/>
+      <c r="G124" s="65"/>
+      <c r="H124" s="65"/>
+      <c r="I124" s="65"/>
     </row>
     <row r="125" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A125" s="53"/>
-      <c r="B125" s="53"/>
+      <c r="A125" s="54"/>
+      <c r="B125" s="54"/>
       <c r="C125" s="49"/>
       <c r="D125" s="48"/>
       <c r="E125" s="48"/>
       <c r="F125" s="35"/>
-      <c r="G125" s="64"/>
-      <c r="H125" s="64"/>
-      <c r="I125" s="64"/>
+      <c r="G125" s="65"/>
+      <c r="H125" s="65"/>
+      <c r="I125" s="65"/>
     </row>
     <row r="126" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A126" s="53"/>
-      <c r="B126" s="53"/>
+      <c r="A126" s="54"/>
+      <c r="B126" s="54"/>
       <c r="C126" s="49"/>
       <c r="D126" s="48"/>
       <c r="E126" s="48"/>
       <c r="F126" s="35"/>
-      <c r="G126" s="64"/>
-      <c r="H126" s="64"/>
-      <c r="I126" s="64"/>
+      <c r="G126" s="65"/>
+      <c r="H126" s="65"/>
+      <c r="I126" s="65"/>
     </row>
     <row r="127" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A127" s="53"/>
-      <c r="B127" s="53"/>
+      <c r="A127" s="54"/>
+      <c r="B127" s="54"/>
       <c r="C127" s="49"/>
       <c r="D127" s="48"/>
       <c r="E127" s="48"/>
       <c r="F127" s="35"/>
-      <c r="G127" s="64"/>
-      <c r="H127" s="64"/>
-      <c r="I127" s="64"/>
+      <c r="G127" s="65"/>
+      <c r="H127" s="65"/>
+      <c r="I127" s="65"/>
     </row>
     <row r="128" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A128" s="53"/>
-      <c r="B128" s="53"/>
+      <c r="A128" s="54"/>
+      <c r="B128" s="54"/>
       <c r="C128" s="49"/>
       <c r="D128" s="48"/>
       <c r="E128" s="48"/>
       <c r="F128" s="35"/>
-      <c r="G128" s="64"/>
-      <c r="H128" s="64"/>
-      <c r="I128" s="64"/>
+      <c r="G128" s="65"/>
+      <c r="H128" s="65"/>
+      <c r="I128" s="65"/>
     </row>
     <row r="129" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A129" s="53"/>
-      <c r="B129" s="53"/>
+      <c r="A129" s="54"/>
+      <c r="B129" s="54"/>
       <c r="C129" s="49"/>
       <c r="D129" s="48"/>
       <c r="E129" s="48"/>
       <c r="F129" s="35"/>
-      <c r="G129" s="64"/>
-      <c r="H129" s="64"/>
-      <c r="I129" s="64"/>
+      <c r="G129" s="65"/>
+      <c r="H129" s="65"/>
+      <c r="I129" s="65"/>
     </row>
     <row r="130" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A130" s="53"/>
-      <c r="B130" s="53"/>
+      <c r="A130" s="54"/>
+      <c r="B130" s="54"/>
       <c r="C130" s="49"/>
       <c r="D130" s="48"/>
       <c r="E130" s="48"/>
       <c r="F130" s="35"/>
-      <c r="G130" s="64"/>
-      <c r="H130" s="64"/>
-      <c r="I130" s="64"/>
+      <c r="G130" s="65"/>
+      <c r="H130" s="65"/>
+      <c r="I130" s="65"/>
     </row>
     <row r="131" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A131" s="53"/>
-      <c r="B131" s="53"/>
+      <c r="A131" s="54"/>
+      <c r="B131" s="54"/>
       <c r="C131" s="49"/>
       <c r="D131" s="48"/>
       <c r="E131" s="48"/>
       <c r="F131" s="35"/>
-      <c r="G131" s="64"/>
-      <c r="H131" s="64"/>
-      <c r="I131" s="64"/>
+      <c r="G131" s="65"/>
+      <c r="H131" s="65"/>
+      <c r="I131" s="65"/>
     </row>
     <row r="132" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A132" s="53"/>
-      <c r="B132" s="53"/>
+      <c r="A132" s="54"/>
+      <c r="B132" s="54"/>
       <c r="C132" s="49"/>
       <c r="D132" s="48"/>
       <c r="E132" s="48"/>
       <c r="F132" s="35"/>
-      <c r="G132" s="64"/>
-      <c r="H132" s="64"/>
-      <c r="I132" s="64"/>
+      <c r="G132" s="65"/>
+      <c r="H132" s="65"/>
+      <c r="I132" s="65"/>
     </row>
     <row r="133" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A133" s="53"/>
-      <c r="B133" s="53"/>
+      <c r="A133" s="54"/>
+      <c r="B133" s="54"/>
       <c r="C133" s="49"/>
       <c r="D133" s="48"/>
       <c r="E133" s="48"/>
       <c r="F133" s="35"/>
-      <c r="G133" s="64"/>
-      <c r="H133" s="64"/>
-      <c r="I133" s="64"/>
+      <c r="G133" s="65"/>
+      <c r="H133" s="65"/>
+      <c r="I133" s="65"/>
     </row>
     <row r="134" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A134" s="53"/>
-      <c r="B134" s="53"/>
+      <c r="A134" s="54"/>
+      <c r="B134" s="54"/>
       <c r="C134" s="49"/>
       <c r="D134" s="48"/>
       <c r="E134" s="48"/>
       <c r="F134" s="35"/>
-      <c r="G134" s="64"/>
-      <c r="H134" s="64"/>
-      <c r="I134" s="64"/>
+      <c r="G134" s="65"/>
+      <c r="H134" s="65"/>
+      <c r="I134" s="65"/>
     </row>
     <row r="135" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A135" s="53"/>
-      <c r="B135" s="53"/>
+      <c r="A135" s="54"/>
+      <c r="B135" s="54"/>
       <c r="C135" s="49"/>
       <c r="D135" s="48"/>
       <c r="E135" s="48"/>
       <c r="F135" s="35"/>
-      <c r="G135" s="64"/>
-      <c r="H135" s="64"/>
-      <c r="I135" s="64"/>
+      <c r="G135" s="65"/>
+      <c r="H135" s="65"/>
+      <c r="I135" s="65"/>
     </row>
     <row r="136" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A136" s="53"/>
-      <c r="B136" s="53"/>
+      <c r="A136" s="54"/>
+      <c r="B136" s="54"/>
       <c r="C136" s="35"/>
       <c r="D136" s="48"/>
       <c r="E136" s="48"/>
       <c r="F136" s="35"/>
-      <c r="G136" s="64"/>
-      <c r="H136" s="64"/>
-      <c r="I136" s="64"/>
+      <c r="G136" s="65"/>
+      <c r="H136" s="65"/>
+      <c r="I136" s="65"/>
     </row>
     <row r="137" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A137" s="53"/>
-      <c r="B137" s="53"/>
+      <c r="A137" s="54"/>
+      <c r="B137" s="54"/>
       <c r="C137" s="35"/>
       <c r="D137" s="48"/>
       <c r="E137" s="48"/>
       <c r="F137" s="35"/>
-      <c r="G137" s="64"/>
-      <c r="H137" s="64"/>
-      <c r="I137" s="64"/>
+      <c r="G137" s="65"/>
+      <c r="H137" s="65"/>
+      <c r="I137" s="65"/>
     </row>
     <row r="138" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A138" s="53"/>
-      <c r="B138" s="53"/>
+      <c r="A138" s="54"/>
+      <c r="B138" s="54"/>
       <c r="C138" s="35"/>
       <c r="D138" s="48"/>
       <c r="E138" s="48"/>
       <c r="F138" s="35"/>
-      <c r="G138" s="64"/>
-      <c r="H138" s="64"/>
-      <c r="I138" s="64" t="str">
+      <c r="G138" s="65"/>
+      <c r="H138" s="65"/>
+      <c r="I138" s="65" t="str">
         <f>I136-I137</f>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A139" s="53"/>
-      <c r="B139" s="53"/>
+      <c r="A139" s="54"/>
+      <c r="B139" s="54"/>
       <c r="C139" s="35"/>
       <c r="D139" s="48"/>
       <c r="E139" s="48"/>
       <c r="F139" s="35"/>
-      <c r="G139" s="64"/>
-      <c r="H139" s="64"/>
-      <c r="I139" s="64"/>
+      <c r="G139" s="65"/>
+      <c r="H139" s="65"/>
+      <c r="I139" s="65"/>
     </row>
     <row r="140" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A140" s="53"/>
-      <c r="B140" s="53"/>
+      <c r="A140" s="54"/>
+      <c r="B140" s="54"/>
       <c r="C140" s="35"/>
       <c r="D140" s="48"/>
       <c r="E140" s="48"/>
       <c r="F140" s="35"/>
-      <c r="G140" s="64"/>
-      <c r="H140" s="64"/>
-      <c r="I140" s="65"/>
+      <c r="G140" s="65"/>
+      <c r="H140" s="65"/>
+      <c r="I140" s="66"/>
     </row>
     <row r="141" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A141" s="53"/>
-      <c r="B141" s="53"/>
+      <c r="A141" s="54"/>
+      <c r="B141" s="54"/>
       <c r="C141" s="35"/>
       <c r="D141" s="48"/>
       <c r="E141" s="48"/>
       <c r="F141" s="35"/>
-      <c r="G141" s="64"/>
-      <c r="H141" s="64"/>
-      <c r="I141" s="64"/>
+      <c r="G141" s="65"/>
+      <c r="H141" s="65"/>
+      <c r="I141" s="65"/>
     </row>
     <row r="142" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A142" s="53"/>
-      <c r="B142" s="53"/>
+      <c r="A142" s="54"/>
+      <c r="B142" s="54"/>
       <c r="C142" s="35"/>
       <c r="D142" s="48"/>
       <c r="E142" s="48"/>
       <c r="F142" s="35"/>
-      <c r="G142" s="64"/>
-      <c r="H142" s="64"/>
-      <c r="I142" s="64"/>
+      <c r="G142" s="65"/>
+      <c r="H142" s="65"/>
+      <c r="I142" s="65"/>
     </row>
     <row r="143" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A143" s="53"/>
-      <c r="B143" s="53"/>
+      <c r="A143" s="54"/>
+      <c r="B143" s="54"/>
       <c r="C143" s="35"/>
       <c r="D143" s="48"/>
       <c r="E143" s="48"/>
       <c r="F143" s="35"/>
-      <c r="G143" s="67"/>
-      <c r="H143" s="67"/>
-      <c r="I143" s="64"/>
+      <c r="G143" s="68"/>
+      <c r="H143" s="68"/>
+      <c r="I143" s="65"/>
     </row>
     <row r="144" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A144" s="53"/>
-      <c r="B144" s="53"/>
+      <c r="A144" s="54"/>
+      <c r="B144" s="54"/>
       <c r="C144" s="35"/>
       <c r="D144" s="48"/>
       <c r="E144" s="48"/>
       <c r="F144" s="35"/>
-      <c r="G144" s="64"/>
-      <c r="H144" s="64"/>
-      <c r="I144" s="64"/>
+      <c r="G144" s="65"/>
+      <c r="H144" s="65"/>
+      <c r="I144" s="65"/>
     </row>
     <row r="145" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A145" s="53"/>
-      <c r="B145" s="53"/>
+      <c r="A145" s="54"/>
+      <c r="B145" s="54"/>
       <c r="C145" s="35"/>
       <c r="D145" s="48"/>
       <c r="E145" s="48"/>
       <c r="F145" s="35"/>
-      <c r="G145" s="64"/>
-      <c r="H145" s="64"/>
-      <c r="I145" s="64"/>
+      <c r="G145" s="65"/>
+      <c r="H145" s="65"/>
+      <c r="I145" s="65"/>
     </row>
     <row r="146" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
       <c r="A146" s="52"/>
@@ -2875,9 +2410,9 @@
       <c r="D146" s="52"/>
       <c r="E146" s="52"/>
       <c r="F146" s="52"/>
-      <c r="G146" s="64"/>
-      <c r="H146" s="64"/>
-      <c r="I146" s="64"/>
+      <c r="G146" s="65"/>
+      <c r="H146" s="65"/>
+      <c r="I146" s="65"/>
     </row>
     <row r="147" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
       <c r="A147" s="52"/>
@@ -2886,1142 +2421,1142 @@
       <c r="D147" s="52"/>
       <c r="E147" s="52"/>
       <c r="F147" s="52"/>
-      <c r="G147" s="64"/>
-      <c r="H147" s="64"/>
-      <c r="I147" s="64"/>
+      <c r="G147" s="65"/>
+      <c r="H147" s="65"/>
+      <c r="I147" s="65"/>
     </row>
     <row r="148" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A148" s="53"/>
-      <c r="B148" s="53"/>
+      <c r="A148" s="54"/>
+      <c r="B148" s="54"/>
       <c r="C148" s="35"/>
       <c r="D148" s="48"/>
       <c r="E148" s="48"/>
       <c r="F148" s="35"/>
-      <c r="G148" s="64"/>
-      <c r="H148" s="64"/>
-      <c r="I148" s="64"/>
+      <c r="G148" s="65"/>
+      <c r="H148" s="65"/>
+      <c r="I148" s="65"/>
     </row>
     <row r="149" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A149" s="53"/>
-      <c r="B149" s="53"/>
+      <c r="A149" s="54"/>
+      <c r="B149" s="54"/>
       <c r="C149" s="35"/>
       <c r="D149" s="48"/>
       <c r="E149" s="48"/>
       <c r="F149" s="35"/>
-      <c r="G149" s="64"/>
-      <c r="H149" s="64"/>
-      <c r="I149" s="64"/>
+      <c r="G149" s="65"/>
+      <c r="H149" s="65"/>
+      <c r="I149" s="65"/>
     </row>
     <row r="150" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A150" s="53"/>
-      <c r="B150" s="53"/>
+      <c r="A150" s="54"/>
+      <c r="B150" s="54"/>
       <c r="C150" s="35"/>
       <c r="D150" s="48"/>
       <c r="E150" s="48"/>
       <c r="F150" s="35"/>
-      <c r="G150" s="64"/>
-      <c r="H150" s="64"/>
-      <c r="I150" s="64"/>
+      <c r="G150" s="65"/>
+      <c r="H150" s="65"/>
+      <c r="I150" s="65"/>
     </row>
     <row r="151" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A151" s="53"/>
-      <c r="B151" s="53"/>
+      <c r="A151" s="54"/>
+      <c r="B151" s="54"/>
       <c r="C151" s="35"/>
       <c r="D151" s="48"/>
       <c r="E151" s="48"/>
       <c r="F151" s="35"/>
-      <c r="G151" s="64"/>
-      <c r="H151" s="64"/>
-      <c r="I151" s="64"/>
+      <c r="G151" s="65"/>
+      <c r="H151" s="65"/>
+      <c r="I151" s="65"/>
     </row>
     <row r="152" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A152" s="53"/>
-      <c r="B152" s="53"/>
+      <c r="A152" s="54"/>
+      <c r="B152" s="54"/>
       <c r="C152" s="35"/>
       <c r="D152" s="48"/>
       <c r="E152" s="48"/>
       <c r="F152" s="35"/>
-      <c r="G152" s="64"/>
-      <c r="H152" s="64"/>
-      <c r="I152" s="64"/>
+      <c r="G152" s="65"/>
+      <c r="H152" s="65"/>
+      <c r="I152" s="65"/>
     </row>
     <row r="153" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A153" s="53"/>
-      <c r="B153" s="53"/>
+      <c r="A153" s="54"/>
+      <c r="B153" s="54"/>
       <c r="C153" s="35"/>
       <c r="D153" s="48"/>
       <c r="E153" s="48"/>
       <c r="F153" s="35"/>
-      <c r="G153" s="64"/>
-      <c r="H153" s="64"/>
-      <c r="I153" s="64"/>
+      <c r="G153" s="65"/>
+      <c r="H153" s="65"/>
+      <c r="I153" s="65"/>
     </row>
     <row r="154" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A154" s="53"/>
-      <c r="B154" s="53"/>
+      <c r="A154" s="54"/>
+      <c r="B154" s="54"/>
       <c r="C154" s="35"/>
       <c r="D154" s="48"/>
       <c r="E154" s="48"/>
       <c r="F154" s="35"/>
-      <c r="G154" s="64"/>
-      <c r="H154" s="64"/>
-      <c r="I154" s="64"/>
+      <c r="G154" s="65"/>
+      <c r="H154" s="65"/>
+      <c r="I154" s="65"/>
     </row>
     <row r="155" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A155" s="53"/>
-      <c r="B155" s="53"/>
+      <c r="A155" s="54"/>
+      <c r="B155" s="54"/>
       <c r="C155" s="35"/>
       <c r="D155" s="48"/>
       <c r="E155" s="48"/>
       <c r="F155" s="35"/>
-      <c r="G155" s="64"/>
-      <c r="H155" s="64"/>
-      <c r="I155" s="64"/>
+      <c r="G155" s="65"/>
+      <c r="H155" s="65"/>
+      <c r="I155" s="65"/>
     </row>
     <row r="156" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A156" s="53"/>
-      <c r="B156" s="53"/>
+      <c r="A156" s="54"/>
+      <c r="B156" s="54"/>
       <c r="C156" s="35"/>
       <c r="D156" s="48"/>
       <c r="E156" s="48"/>
       <c r="F156" s="35"/>
-      <c r="G156" s="64"/>
-      <c r="H156" s="64"/>
-      <c r="I156" s="64"/>
+      <c r="G156" s="65"/>
+      <c r="H156" s="65"/>
+      <c r="I156" s="65"/>
     </row>
     <row r="157" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A157" s="53"/>
-      <c r="B157" s="53"/>
+      <c r="A157" s="54"/>
+      <c r="B157" s="54"/>
       <c r="C157" s="35"/>
       <c r="D157" s="48"/>
       <c r="E157" s="48"/>
       <c r="F157" s="35"/>
-      <c r="G157" s="64"/>
-      <c r="H157" s="64"/>
-      <c r="I157" s="64"/>
+      <c r="G157" s="65"/>
+      <c r="H157" s="65"/>
+      <c r="I157" s="65"/>
     </row>
     <row r="158" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A158" s="53"/>
-      <c r="B158" s="53"/>
+      <c r="A158" s="54"/>
+      <c r="B158" s="54"/>
       <c r="C158" s="35"/>
       <c r="D158" s="48"/>
       <c r="E158" s="48"/>
       <c r="F158" s="35"/>
-      <c r="G158" s="64"/>
-      <c r="H158" s="64"/>
-      <c r="I158" s="64"/>
+      <c r="G158" s="65"/>
+      <c r="H158" s="65"/>
+      <c r="I158" s="65"/>
     </row>
     <row r="159" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A159" s="53"/>
-      <c r="B159" s="53"/>
+      <c r="A159" s="54"/>
+      <c r="B159" s="54"/>
       <c r="C159" s="35"/>
       <c r="D159" s="48"/>
       <c r="E159" s="48"/>
       <c r="F159" s="35"/>
-      <c r="G159" s="64"/>
-      <c r="H159" s="64"/>
-      <c r="I159" s="64"/>
+      <c r="G159" s="65"/>
+      <c r="H159" s="65"/>
+      <c r="I159" s="65"/>
     </row>
     <row r="160" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A160" s="53"/>
-      <c r="B160" s="53"/>
+      <c r="A160" s="54"/>
+      <c r="B160" s="54"/>
       <c r="C160" s="35"/>
       <c r="D160" s="48"/>
       <c r="E160" s="48"/>
       <c r="F160" s="35"/>
-      <c r="G160" s="64"/>
-      <c r="H160" s="64"/>
-      <c r="I160" s="64"/>
+      <c r="G160" s="65"/>
+      <c r="H160" s="65"/>
+      <c r="I160" s="65"/>
     </row>
     <row r="161" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A161" s="53"/>
-      <c r="B161" s="53"/>
+      <c r="A161" s="54"/>
+      <c r="B161" s="54"/>
       <c r="C161" s="35"/>
       <c r="D161" s="48"/>
       <c r="E161" s="48"/>
       <c r="F161" s="35"/>
-      <c r="G161" s="64"/>
-      <c r="H161" s="64"/>
-      <c r="I161" s="64"/>
+      <c r="G161" s="65"/>
+      <c r="H161" s="65"/>
+      <c r="I161" s="65"/>
     </row>
     <row r="162" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A162" s="53"/>
-      <c r="B162" s="53"/>
+      <c r="A162" s="54"/>
+      <c r="B162" s="54"/>
       <c r="C162" s="35"/>
       <c r="D162" s="48"/>
       <c r="E162" s="48"/>
       <c r="F162" s="35"/>
-      <c r="G162" s="64"/>
-      <c r="H162" s="64"/>
-      <c r="I162" s="64"/>
+      <c r="G162" s="65"/>
+      <c r="H162" s="65"/>
+      <c r="I162" s="65"/>
     </row>
     <row r="163" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A163" s="53"/>
-      <c r="B163" s="53"/>
+      <c r="A163" s="54"/>
+      <c r="B163" s="54"/>
       <c r="C163" s="35"/>
       <c r="D163" s="48"/>
       <c r="E163" s="48"/>
       <c r="F163" s="35"/>
-      <c r="G163" s="64"/>
-      <c r="H163" s="64"/>
-      <c r="I163" s="64"/>
+      <c r="G163" s="65"/>
+      <c r="H163" s="65"/>
+      <c r="I163" s="65"/>
     </row>
     <row r="164" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A164" s="53"/>
-      <c r="B164" s="53"/>
+      <c r="A164" s="54"/>
+      <c r="B164" s="54"/>
       <c r="C164" s="35"/>
       <c r="D164" s="48"/>
       <c r="E164" s="48"/>
       <c r="F164" s="35"/>
-      <c r="G164" s="64"/>
-      <c r="H164" s="64"/>
-      <c r="I164" s="64"/>
+      <c r="G164" s="65"/>
+      <c r="H164" s="65"/>
+      <c r="I164" s="65"/>
     </row>
     <row r="165" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A165" s="53"/>
-      <c r="B165" s="53"/>
+      <c r="A165" s="54"/>
+      <c r="B165" s="54"/>
       <c r="C165" s="35"/>
       <c r="D165" s="48"/>
       <c r="E165" s="48"/>
       <c r="F165" s="48"/>
-      <c r="G165" s="64"/>
-      <c r="H165" s="64"/>
-      <c r="I165" s="64"/>
+      <c r="G165" s="65"/>
+      <c r="H165" s="65"/>
+      <c r="I165" s="65"/>
     </row>
     <row r="166" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A166" s="53"/>
-      <c r="B166" s="53"/>
+      <c r="A166" s="54"/>
+      <c r="B166" s="54"/>
       <c r="C166" s="35"/>
       <c r="D166" s="48"/>
       <c r="E166" s="48"/>
       <c r="F166" s="48"/>
-      <c r="G166" s="64"/>
-      <c r="H166" s="64"/>
-      <c r="I166" s="64"/>
+      <c r="G166" s="65"/>
+      <c r="H166" s="65"/>
+      <c r="I166" s="65"/>
     </row>
     <row r="167" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A167" s="53"/>
-      <c r="B167" s="53"/>
+      <c r="A167" s="54"/>
+      <c r="B167" s="54"/>
       <c r="C167" s="35"/>
       <c r="D167" s="48"/>
       <c r="E167" s="48"/>
       <c r="F167" s="35"/>
-      <c r="G167" s="64"/>
-      <c r="H167" s="64"/>
-      <c r="I167" s="64"/>
+      <c r="G167" s="65"/>
+      <c r="H167" s="65"/>
+      <c r="I167" s="65"/>
     </row>
     <row r="168" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A168" s="53"/>
-      <c r="B168" s="53"/>
+      <c r="A168" s="54"/>
+      <c r="B168" s="54"/>
       <c r="C168" s="35"/>
       <c r="D168" s="48"/>
       <c r="E168" s="48"/>
       <c r="F168" s="35"/>
-      <c r="G168" s="64"/>
-      <c r="H168" s="64"/>
-      <c r="I168" s="64"/>
+      <c r="G168" s="65"/>
+      <c r="H168" s="65"/>
+      <c r="I168" s="65"/>
     </row>
     <row r="169" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A169" s="53"/>
-      <c r="B169" s="53"/>
+      <c r="A169" s="54"/>
+      <c r="B169" s="54"/>
       <c r="C169" s="35"/>
       <c r="D169" s="48"/>
       <c r="E169" s="48"/>
       <c r="F169" s="35"/>
-      <c r="G169" s="64"/>
-      <c r="H169" s="64"/>
-      <c r="I169" s="64"/>
+      <c r="G169" s="65"/>
+      <c r="H169" s="65"/>
+      <c r="I169" s="65"/>
     </row>
     <row r="170" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A170" s="53"/>
-      <c r="B170" s="53"/>
+      <c r="A170" s="54"/>
+      <c r="B170" s="54"/>
       <c r="C170" s="35"/>
       <c r="D170" s="48"/>
       <c r="E170" s="48"/>
       <c r="F170" s="35"/>
-      <c r="G170" s="64"/>
-      <c r="H170" s="64"/>
-      <c r="I170" s="64"/>
+      <c r="G170" s="65"/>
+      <c r="H170" s="65"/>
+      <c r="I170" s="65"/>
     </row>
     <row r="171" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A171" s="53"/>
-      <c r="B171" s="53"/>
+      <c r="A171" s="54"/>
+      <c r="B171" s="54"/>
       <c r="C171" s="35"/>
       <c r="D171" s="48"/>
       <c r="E171" s="48"/>
       <c r="F171" s="35"/>
-      <c r="G171" s="64"/>
-      <c r="H171" s="64"/>
-      <c r="I171" s="64"/>
+      <c r="G171" s="65"/>
+      <c r="H171" s="65"/>
+      <c r="I171" s="65"/>
     </row>
     <row r="172" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A172" s="53"/>
-      <c r="B172" s="53"/>
+      <c r="A172" s="54"/>
+      <c r="B172" s="54"/>
       <c r="C172" s="35"/>
       <c r="D172" s="48"/>
       <c r="E172" s="48"/>
       <c r="F172" s="35"/>
-      <c r="G172" s="64"/>
-      <c r="H172" s="64"/>
-      <c r="I172" s="64"/>
+      <c r="G172" s="65"/>
+      <c r="H172" s="65"/>
+      <c r="I172" s="65"/>
     </row>
     <row r="173" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A173" s="53"/>
-      <c r="B173" s="53"/>
+      <c r="A173" s="54"/>
+      <c r="B173" s="54"/>
       <c r="C173" s="35"/>
       <c r="D173" s="48"/>
       <c r="E173" s="48"/>
       <c r="F173" s="35"/>
-      <c r="G173" s="64"/>
-      <c r="H173" s="64"/>
-      <c r="I173" s="64"/>
+      <c r="G173" s="65"/>
+      <c r="H173" s="65"/>
+      <c r="I173" s="65"/>
     </row>
     <row r="174" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A174" s="53"/>
-      <c r="B174" s="53"/>
+      <c r="A174" s="54"/>
+      <c r="B174" s="54"/>
       <c r="C174" s="35"/>
       <c r="D174" s="48"/>
       <c r="E174" s="48"/>
       <c r="F174" s="35"/>
-      <c r="G174" s="64"/>
-      <c r="H174" s="64"/>
-      <c r="I174" s="64"/>
+      <c r="G174" s="65"/>
+      <c r="H174" s="65"/>
+      <c r="I174" s="65"/>
     </row>
     <row r="175" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A175" s="53"/>
-      <c r="B175" s="53"/>
+      <c r="A175" s="54"/>
+      <c r="B175" s="54"/>
       <c r="C175" s="35"/>
       <c r="D175" s="48"/>
       <c r="E175" s="48"/>
       <c r="F175" s="35"/>
-      <c r="G175" s="64"/>
-      <c r="H175" s="64"/>
-      <c r="I175" s="64"/>
+      <c r="G175" s="65"/>
+      <c r="H175" s="65"/>
+      <c r="I175" s="65"/>
     </row>
     <row r="176" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A176" s="53"/>
-      <c r="B176" s="53"/>
+      <c r="A176" s="54"/>
+      <c r="B176" s="54"/>
       <c r="C176" s="35"/>
       <c r="D176" s="48"/>
       <c r="E176" s="48"/>
       <c r="F176" s="35"/>
-      <c r="G176" s="64"/>
-      <c r="H176" s="64"/>
-      <c r="I176" s="64"/>
+      <c r="G176" s="65"/>
+      <c r="H176" s="65"/>
+      <c r="I176" s="65"/>
     </row>
     <row r="177" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A177" s="53"/>
-      <c r="B177" s="53"/>
+      <c r="A177" s="54"/>
+      <c r="B177" s="54"/>
       <c r="C177" s="35"/>
       <c r="D177" s="48"/>
       <c r="E177" s="48"/>
       <c r="F177" s="35"/>
-      <c r="G177" s="64"/>
-      <c r="H177" s="64"/>
-      <c r="I177" s="64"/>
+      <c r="G177" s="65"/>
+      <c r="H177" s="65"/>
+      <c r="I177" s="65"/>
     </row>
     <row r="178" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A178" s="53"/>
-      <c r="B178" s="53"/>
+      <c r="A178" s="54"/>
+      <c r="B178" s="54"/>
       <c r="C178" s="35"/>
       <c r="D178" s="48"/>
       <c r="E178" s="48"/>
       <c r="F178" s="35"/>
-      <c r="G178" s="64"/>
-      <c r="H178" s="64"/>
-      <c r="I178" s="64"/>
+      <c r="G178" s="65"/>
+      <c r="H178" s="65"/>
+      <c r="I178" s="65"/>
     </row>
     <row r="179" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A179" s="53"/>
-      <c r="B179" s="53"/>
+      <c r="A179" s="54"/>
+      <c r="B179" s="54"/>
       <c r="C179" s="35"/>
       <c r="D179" s="48"/>
       <c r="E179" s="48"/>
       <c r="F179" s="35"/>
-      <c r="G179" s="64"/>
-      <c r="H179" s="64"/>
-      <c r="I179" s="64"/>
+      <c r="G179" s="65"/>
+      <c r="H179" s="65"/>
+      <c r="I179" s="65"/>
     </row>
     <row r="180" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A180" s="53"/>
-      <c r="B180" s="53"/>
+      <c r="A180" s="54"/>
+      <c r="B180" s="54"/>
       <c r="C180" s="35"/>
       <c r="D180" s="48"/>
       <c r="E180" s="48"/>
       <c r="F180" s="35"/>
-      <c r="G180" s="64"/>
-      <c r="H180" s="64"/>
-      <c r="I180" s="64"/>
+      <c r="G180" s="65"/>
+      <c r="H180" s="65"/>
+      <c r="I180" s="65"/>
     </row>
     <row r="181" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A181" s="53"/>
-      <c r="B181" s="53"/>
+      <c r="A181" s="54"/>
+      <c r="B181" s="54"/>
       <c r="C181" s="35"/>
       <c r="D181" s="48"/>
       <c r="E181" s="48"/>
       <c r="F181" s="35"/>
-      <c r="G181" s="64"/>
-      <c r="H181" s="64"/>
-      <c r="I181" s="64"/>
+      <c r="G181" s="65"/>
+      <c r="H181" s="65"/>
+      <c r="I181" s="65"/>
     </row>
     <row r="182" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A182" s="53"/>
-      <c r="B182" s="53"/>
+      <c r="A182" s="54"/>
+      <c r="B182" s="54"/>
       <c r="C182" s="35"/>
       <c r="D182" s="48"/>
       <c r="E182" s="48"/>
       <c r="F182" s="35"/>
-      <c r="G182" s="64"/>
-      <c r="H182" s="64"/>
-      <c r="I182" s="64"/>
+      <c r="G182" s="65"/>
+      <c r="H182" s="65"/>
+      <c r="I182" s="65"/>
     </row>
     <row r="183" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A183" s="53"/>
-      <c r="B183" s="53"/>
+      <c r="A183" s="54"/>
+      <c r="B183" s="54"/>
       <c r="C183" s="35"/>
       <c r="D183" s="48"/>
       <c r="E183" s="48"/>
       <c r="F183" s="35"/>
-      <c r="G183" s="64"/>
-      <c r="H183" s="64"/>
-      <c r="I183" s="64"/>
+      <c r="G183" s="65"/>
+      <c r="H183" s="65"/>
+      <c r="I183" s="65"/>
     </row>
     <row r="184" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A184" s="53"/>
-      <c r="B184" s="53"/>
+      <c r="A184" s="54"/>
+      <c r="B184" s="54"/>
       <c r="C184" s="35"/>
       <c r="D184" s="48"/>
       <c r="E184" s="48"/>
       <c r="F184" s="35"/>
-      <c r="G184" s="64"/>
-      <c r="H184" s="64"/>
-      <c r="I184" s="64"/>
+      <c r="G184" s="65"/>
+      <c r="H184" s="65"/>
+      <c r="I184" s="65"/>
     </row>
     <row r="185" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A185" s="53"/>
-      <c r="B185" s="53"/>
+      <c r="A185" s="54"/>
+      <c r="B185" s="54"/>
       <c r="C185" s="35"/>
       <c r="D185" s="48"/>
       <c r="E185" s="48"/>
       <c r="F185" s="35"/>
-      <c r="G185" s="64"/>
-      <c r="H185" s="64"/>
-      <c r="I185" s="64"/>
+      <c r="G185" s="65"/>
+      <c r="H185" s="65"/>
+      <c r="I185" s="65"/>
     </row>
     <row r="186" spans="1:10" customHeight="1" ht="39.75" s="8" customFormat="1">
-      <c r="A186" s="53"/>
-      <c r="B186" s="53"/>
+      <c r="A186" s="54"/>
+      <c r="B186" s="54"/>
       <c r="C186" s="35"/>
       <c r="D186" s="48"/>
       <c r="E186" s="48"/>
       <c r="F186" s="35"/>
-      <c r="G186" s="64"/>
-      <c r="H186" s="64"/>
-      <c r="I186" s="64"/>
+      <c r="G186" s="65"/>
+      <c r="H186" s="65"/>
+      <c r="I186" s="65"/>
     </row>
     <row r="187" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A187" s="53"/>
-      <c r="B187" s="53"/>
+      <c r="A187" s="54"/>
+      <c r="B187" s="54"/>
       <c r="C187" s="35"/>
       <c r="D187" s="48"/>
       <c r="E187" s="48"/>
       <c r="F187" s="35"/>
-      <c r="G187" s="64"/>
-      <c r="H187" s="64"/>
-      <c r="I187" s="64"/>
+      <c r="G187" s="65"/>
+      <c r="H187" s="65"/>
+      <c r="I187" s="65"/>
     </row>
     <row r="188" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A188" s="53"/>
-      <c r="B188" s="53"/>
+      <c r="A188" s="54"/>
+      <c r="B188" s="54"/>
       <c r="C188" s="35"/>
       <c r="D188" s="48"/>
       <c r="E188" s="48"/>
       <c r="F188" s="48"/>
-      <c r="G188" s="64"/>
-      <c r="H188" s="64"/>
-      <c r="I188" s="64"/>
+      <c r="G188" s="65"/>
+      <c r="H188" s="65"/>
+      <c r="I188" s="65"/>
     </row>
     <row r="189" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A189" s="53"/>
-      <c r="B189" s="53"/>
+      <c r="A189" s="54"/>
+      <c r="B189" s="54"/>
       <c r="C189" s="48"/>
       <c r="D189" s="48"/>
       <c r="E189" s="48"/>
       <c r="F189" s="48"/>
-      <c r="G189" s="64"/>
-      <c r="H189" s="64"/>
-      <c r="I189" s="64"/>
+      <c r="G189" s="65"/>
+      <c r="H189" s="65"/>
+      <c r="I189" s="65"/>
     </row>
     <row r="190" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A190" s="53"/>
-      <c r="B190" s="53"/>
+      <c r="A190" s="54"/>
+      <c r="B190" s="54"/>
       <c r="C190" s="35"/>
       <c r="D190" s="48"/>
       <c r="E190" s="48"/>
       <c r="F190" s="35"/>
-      <c r="G190" s="64"/>
-      <c r="H190" s="64"/>
-      <c r="I190" s="64"/>
+      <c r="G190" s="65"/>
+      <c r="H190" s="65"/>
+      <c r="I190" s="65"/>
     </row>
     <row r="191" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A191" s="53"/>
-      <c r="B191" s="53"/>
+      <c r="A191" s="54"/>
+      <c r="B191" s="54"/>
       <c r="C191" s="35"/>
       <c r="D191" s="48"/>
       <c r="E191" s="48"/>
       <c r="F191" s="35"/>
-      <c r="G191" s="64"/>
-      <c r="H191" s="64"/>
-      <c r="I191" s="67"/>
+      <c r="G191" s="65"/>
+      <c r="H191" s="65"/>
+      <c r="I191" s="68"/>
     </row>
     <row r="192" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A192" s="53"/>
-      <c r="B192" s="53"/>
+      <c r="A192" s="54"/>
+      <c r="B192" s="54"/>
       <c r="C192" s="35"/>
       <c r="D192" s="48"/>
       <c r="E192" s="48"/>
       <c r="F192" s="35"/>
-      <c r="G192" s="64"/>
-      <c r="H192" s="64"/>
-      <c r="I192" s="64"/>
+      <c r="G192" s="65"/>
+      <c r="H192" s="65"/>
+      <c r="I192" s="65"/>
     </row>
     <row r="193" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A193" s="53"/>
-      <c r="B193" s="53"/>
+      <c r="A193" s="54"/>
+      <c r="B193" s="54"/>
       <c r="C193" s="35"/>
       <c r="D193" s="48"/>
       <c r="E193" s="48"/>
       <c r="F193" s="35"/>
-      <c r="G193" s="64"/>
-      <c r="H193" s="64"/>
-      <c r="I193" s="64"/>
+      <c r="G193" s="65"/>
+      <c r="H193" s="65"/>
+      <c r="I193" s="65"/>
     </row>
     <row r="194" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A194" s="53"/>
-      <c r="B194" s="53"/>
+      <c r="A194" s="54"/>
+      <c r="B194" s="54"/>
       <c r="C194" s="35"/>
       <c r="D194" s="48"/>
       <c r="E194" s="48"/>
       <c r="F194" s="35"/>
-      <c r="G194" s="64"/>
-      <c r="H194" s="64"/>
-      <c r="I194" s="64"/>
+      <c r="G194" s="65"/>
+      <c r="H194" s="65"/>
+      <c r="I194" s="65"/>
     </row>
     <row r="195" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A195" s="53"/>
-      <c r="B195" s="53"/>
+      <c r="A195" s="54"/>
+      <c r="B195" s="54"/>
       <c r="C195" s="35"/>
       <c r="D195" s="48"/>
       <c r="E195" s="48"/>
       <c r="F195" s="35"/>
-      <c r="G195" s="64"/>
-      <c r="H195" s="64"/>
-      <c r="I195" s="64"/>
+      <c r="G195" s="65"/>
+      <c r="H195" s="65"/>
+      <c r="I195" s="65"/>
     </row>
     <row r="196" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A196" s="56"/>
-      <c r="B196" s="56"/>
+      <c r="A196" s="57"/>
+      <c r="B196" s="57"/>
       <c r="C196" s="49"/>
       <c r="D196" s="47"/>
       <c r="E196" s="47"/>
       <c r="F196" s="35"/>
-      <c r="G196" s="64"/>
-      <c r="H196" s="64"/>
-      <c r="I196" s="64"/>
+      <c r="G196" s="65"/>
+      <c r="H196" s="65"/>
+      <c r="I196" s="65"/>
     </row>
     <row r="197" spans="1:10" customHeight="1" ht="39.75" s="9" customFormat="1">
-      <c r="A197" s="53"/>
-      <c r="B197" s="53"/>
-      <c r="C197" s="57"/>
+      <c r="A197" s="54"/>
+      <c r="B197" s="54"/>
+      <c r="C197" s="58"/>
       <c r="D197" s="48"/>
       <c r="E197" s="48"/>
       <c r="F197" s="35"/>
-      <c r="G197" s="64"/>
-      <c r="H197" s="64"/>
-      <c r="I197" s="64"/>
+      <c r="G197" s="65"/>
+      <c r="H197" s="65"/>
+      <c r="I197" s="65"/>
     </row>
     <row r="198" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A198" s="53"/>
-      <c r="B198" s="53"/>
+      <c r="A198" s="54"/>
+      <c r="B198" s="54"/>
       <c r="C198" s="35"/>
       <c r="D198" s="48"/>
       <c r="E198" s="48"/>
       <c r="F198" s="35"/>
-      <c r="G198" s="64"/>
-      <c r="H198" s="64"/>
-      <c r="I198" s="64"/>
+      <c r="G198" s="65"/>
+      <c r="H198" s="65"/>
+      <c r="I198" s="65"/>
     </row>
     <row r="199" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A199" s="53"/>
-      <c r="B199" s="53"/>
+      <c r="A199" s="54"/>
+      <c r="B199" s="54"/>
       <c r="C199" s="35"/>
       <c r="D199" s="48"/>
       <c r="E199" s="48"/>
       <c r="F199" s="35"/>
-      <c r="G199" s="64"/>
-      <c r="H199" s="64"/>
-      <c r="I199" s="64"/>
+      <c r="G199" s="65"/>
+      <c r="H199" s="65"/>
+      <c r="I199" s="65"/>
     </row>
     <row r="200" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A200" s="53"/>
-      <c r="B200" s="53"/>
+      <c r="A200" s="54"/>
+      <c r="B200" s="54"/>
       <c r="C200" s="35"/>
       <c r="D200" s="48"/>
       <c r="E200" s="48"/>
       <c r="F200" s="35"/>
-      <c r="G200" s="64"/>
-      <c r="H200" s="64"/>
-      <c r="I200" s="64"/>
+      <c r="G200" s="65"/>
+      <c r="H200" s="65"/>
+      <c r="I200" s="65"/>
     </row>
     <row r="201" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A201" s="53"/>
-      <c r="B201" s="53"/>
+      <c r="A201" s="54"/>
+      <c r="B201" s="54"/>
       <c r="C201" s="35"/>
       <c r="D201" s="48"/>
       <c r="E201" s="48"/>
       <c r="F201" s="35"/>
-      <c r="G201" s="64"/>
-      <c r="H201" s="64"/>
-      <c r="I201" s="64"/>
+      <c r="G201" s="65"/>
+      <c r="H201" s="65"/>
+      <c r="I201" s="65"/>
     </row>
     <row r="202" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A202" s="53"/>
-      <c r="B202" s="53"/>
+      <c r="A202" s="54"/>
+      <c r="B202" s="54"/>
       <c r="C202" s="35"/>
       <c r="D202" s="48"/>
       <c r="E202" s="48"/>
       <c r="F202" s="35"/>
-      <c r="G202" s="64"/>
-      <c r="H202" s="64"/>
-      <c r="I202" s="64"/>
+      <c r="G202" s="65"/>
+      <c r="H202" s="65"/>
+      <c r="I202" s="65"/>
     </row>
     <row r="203" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A203" s="53"/>
-      <c r="B203" s="53"/>
+      <c r="A203" s="54"/>
+      <c r="B203" s="54"/>
       <c r="C203" s="35"/>
       <c r="D203" s="48"/>
       <c r="E203" s="48"/>
       <c r="F203" s="35"/>
-      <c r="G203" s="64"/>
-      <c r="H203" s="64"/>
-      <c r="I203" s="64"/>
+      <c r="G203" s="65"/>
+      <c r="H203" s="65"/>
+      <c r="I203" s="65"/>
     </row>
     <row r="204" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A204" s="53"/>
-      <c r="B204" s="53"/>
+      <c r="A204" s="54"/>
+      <c r="B204" s="54"/>
       <c r="C204" s="35"/>
       <c r="D204" s="48"/>
       <c r="E204" s="48"/>
       <c r="F204" s="35"/>
-      <c r="G204" s="64"/>
-      <c r="H204" s="64"/>
-      <c r="I204" s="64"/>
+      <c r="G204" s="65"/>
+      <c r="H204" s="65"/>
+      <c r="I204" s="65"/>
     </row>
     <row r="205" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A205" s="53"/>
-      <c r="B205" s="53"/>
+      <c r="A205" s="54"/>
+      <c r="B205" s="54"/>
       <c r="C205" s="35"/>
       <c r="D205" s="48"/>
       <c r="E205" s="48"/>
       <c r="F205" s="35"/>
-      <c r="G205" s="64"/>
-      <c r="H205" s="64"/>
-      <c r="I205" s="64"/>
+      <c r="G205" s="65"/>
+      <c r="H205" s="65"/>
+      <c r="I205" s="65"/>
     </row>
     <row r="206" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A206" s="53"/>
-      <c r="B206" s="53"/>
+      <c r="A206" s="54"/>
+      <c r="B206" s="54"/>
       <c r="C206" s="35"/>
       <c r="D206" s="48"/>
       <c r="E206" s="48"/>
       <c r="F206" s="35"/>
-      <c r="G206" s="64"/>
-      <c r="H206" s="64"/>
-      <c r="I206" s="64"/>
+      <c r="G206" s="65"/>
+      <c r="H206" s="65"/>
+      <c r="I206" s="65"/>
     </row>
     <row r="207" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A207" s="53"/>
-      <c r="B207" s="53"/>
+      <c r="A207" s="54"/>
+      <c r="B207" s="54"/>
       <c r="C207" s="35"/>
       <c r="D207" s="48"/>
       <c r="E207" s="48"/>
       <c r="F207" s="35"/>
-      <c r="G207" s="64"/>
-      <c r="H207" s="64"/>
-      <c r="I207" s="64"/>
+      <c r="G207" s="65"/>
+      <c r="H207" s="65"/>
+      <c r="I207" s="65"/>
     </row>
     <row r="208" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A208" s="53"/>
-      <c r="B208" s="53"/>
+      <c r="A208" s="54"/>
+      <c r="B208" s="54"/>
       <c r="C208" s="48"/>
       <c r="D208" s="48"/>
       <c r="E208" s="48"/>
       <c r="F208" s="48"/>
-      <c r="G208" s="64"/>
-      <c r="H208" s="64"/>
-      <c r="I208" s="64"/>
+      <c r="G208" s="65"/>
+      <c r="H208" s="65"/>
+      <c r="I208" s="65"/>
     </row>
     <row r="209" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A209" s="53"/>
-      <c r="B209" s="53"/>
+      <c r="A209" s="54"/>
+      <c r="B209" s="54"/>
       <c r="C209" s="48"/>
       <c r="D209" s="48"/>
       <c r="E209" s="48"/>
       <c r="F209" s="48"/>
-      <c r="G209" s="64"/>
-      <c r="H209" s="64"/>
-      <c r="I209" s="64"/>
+      <c r="G209" s="65"/>
+      <c r="H209" s="65"/>
+      <c r="I209" s="65"/>
     </row>
     <row r="210" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A210" s="53"/>
-      <c r="B210" s="53"/>
+      <c r="A210" s="54"/>
+      <c r="B210" s="54"/>
       <c r="C210" s="35"/>
       <c r="D210" s="48"/>
       <c r="E210" s="48"/>
       <c r="F210" s="35"/>
-      <c r="G210" s="64"/>
-      <c r="H210" s="64"/>
-      <c r="I210" s="64"/>
+      <c r="G210" s="65"/>
+      <c r="H210" s="65"/>
+      <c r="I210" s="65"/>
     </row>
     <row r="211" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A211" s="53"/>
-      <c r="B211" s="53"/>
+      <c r="A211" s="54"/>
+      <c r="B211" s="54"/>
       <c r="C211" s="35"/>
       <c r="D211" s="48"/>
       <c r="E211" s="48"/>
       <c r="F211" s="35"/>
-      <c r="G211" s="64"/>
-      <c r="H211" s="64"/>
-      <c r="I211" s="64"/>
+      <c r="G211" s="65"/>
+      <c r="H211" s="65"/>
+      <c r="I211" s="65"/>
     </row>
     <row r="212" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A212" s="53"/>
-      <c r="B212" s="53"/>
+      <c r="A212" s="54"/>
+      <c r="B212" s="54"/>
       <c r="C212" s="35"/>
       <c r="D212" s="48"/>
       <c r="E212" s="48"/>
       <c r="F212" s="35"/>
-      <c r="G212" s="64"/>
-      <c r="H212" s="64"/>
-      <c r="I212" s="64"/>
+      <c r="G212" s="65"/>
+      <c r="H212" s="65"/>
+      <c r="I212" s="65"/>
     </row>
     <row r="213" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A213" s="53"/>
-      <c r="B213" s="53"/>
+      <c r="A213" s="54"/>
+      <c r="B213" s="54"/>
       <c r="C213" s="35"/>
       <c r="D213" s="48"/>
       <c r="E213" s="48"/>
       <c r="F213" s="35"/>
-      <c r="G213" s="64"/>
-      <c r="H213" s="64"/>
-      <c r="I213" s="64"/>
+      <c r="G213" s="65"/>
+      <c r="H213" s="65"/>
+      <c r="I213" s="65"/>
     </row>
     <row r="214" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A214" s="53"/>
-      <c r="B214" s="53"/>
+      <c r="A214" s="54"/>
+      <c r="B214" s="54"/>
       <c r="C214" s="35"/>
       <c r="D214" s="48"/>
       <c r="E214" s="48"/>
       <c r="F214" s="35"/>
-      <c r="G214" s="64"/>
-      <c r="H214" s="64"/>
-      <c r="I214" s="64"/>
+      <c r="G214" s="65"/>
+      <c r="H214" s="65"/>
+      <c r="I214" s="65"/>
     </row>
     <row r="215" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A215" s="53"/>
-      <c r="B215" s="53"/>
+      <c r="A215" s="54"/>
+      <c r="B215" s="54"/>
       <c r="C215" s="35"/>
       <c r="D215" s="48"/>
       <c r="E215" s="48"/>
       <c r="F215" s="35"/>
-      <c r="G215" s="64"/>
-      <c r="H215" s="64"/>
-      <c r="I215" s="64"/>
+      <c r="G215" s="65"/>
+      <c r="H215" s="65"/>
+      <c r="I215" s="65"/>
     </row>
     <row r="216" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A216" s="53"/>
-      <c r="B216" s="53"/>
+      <c r="A216" s="54"/>
+      <c r="B216" s="54"/>
       <c r="C216" s="35"/>
       <c r="D216" s="48"/>
       <c r="E216" s="48"/>
       <c r="F216" s="35"/>
-      <c r="G216" s="64"/>
-      <c r="H216" s="64"/>
-      <c r="I216" s="64"/>
+      <c r="G216" s="65"/>
+      <c r="H216" s="65"/>
+      <c r="I216" s="65"/>
     </row>
     <row r="217" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A217" s="53"/>
-      <c r="B217" s="53"/>
+      <c r="A217" s="54"/>
+      <c r="B217" s="54"/>
       <c r="C217" s="35"/>
       <c r="D217" s="48"/>
       <c r="E217" s="48"/>
       <c r="F217" s="35"/>
-      <c r="G217" s="64"/>
-      <c r="H217" s="64"/>
-      <c r="I217" s="64"/>
+      <c r="G217" s="65"/>
+      <c r="H217" s="65"/>
+      <c r="I217" s="65"/>
     </row>
     <row r="218" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A218" s="53"/>
-      <c r="B218" s="53"/>
+      <c r="A218" s="54"/>
+      <c r="B218" s="54"/>
       <c r="C218" s="35"/>
       <c r="D218" s="48"/>
       <c r="E218" s="48"/>
       <c r="F218" s="35"/>
-      <c r="G218" s="64"/>
-      <c r="H218" s="64"/>
-      <c r="I218" s="64"/>
+      <c r="G218" s="65"/>
+      <c r="H218" s="65"/>
+      <c r="I218" s="65"/>
     </row>
     <row r="219" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A219" s="53"/>
-      <c r="B219" s="53"/>
+      <c r="A219" s="54"/>
+      <c r="B219" s="54"/>
       <c r="C219" s="35"/>
       <c r="D219" s="48"/>
       <c r="E219" s="48"/>
       <c r="F219" s="35"/>
-      <c r="G219" s="64"/>
-      <c r="H219" s="64"/>
-      <c r="I219" s="64"/>
+      <c r="G219" s="65"/>
+      <c r="H219" s="65"/>
+      <c r="I219" s="65"/>
     </row>
     <row r="220" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A220" s="53"/>
-      <c r="B220" s="53"/>
+      <c r="A220" s="54"/>
+      <c r="B220" s="54"/>
       <c r="C220" s="35"/>
       <c r="D220" s="48"/>
       <c r="E220" s="48"/>
       <c r="F220" s="35"/>
-      <c r="G220" s="64"/>
-      <c r="H220" s="64"/>
-      <c r="I220" s="64"/>
+      <c r="G220" s="65"/>
+      <c r="H220" s="65"/>
+      <c r="I220" s="65"/>
     </row>
     <row r="221" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A221" s="53"/>
-      <c r="B221" s="53"/>
+      <c r="A221" s="54"/>
+      <c r="B221" s="54"/>
       <c r="C221" s="35"/>
       <c r="D221" s="48"/>
       <c r="E221" s="48"/>
       <c r="F221" s="35"/>
-      <c r="G221" s="64"/>
-      <c r="H221" s="64"/>
-      <c r="I221" s="64"/>
+      <c r="G221" s="65"/>
+      <c r="H221" s="65"/>
+      <c r="I221" s="65"/>
     </row>
     <row r="222" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A222" s="53"/>
-      <c r="B222" s="53"/>
+      <c r="A222" s="54"/>
+      <c r="B222" s="54"/>
       <c r="C222" s="35"/>
       <c r="D222" s="48"/>
       <c r="E222" s="48"/>
       <c r="F222" s="35"/>
-      <c r="G222" s="64"/>
-      <c r="H222" s="64"/>
-      <c r="I222" s="64"/>
+      <c r="G222" s="65"/>
+      <c r="H222" s="65"/>
+      <c r="I222" s="65"/>
     </row>
     <row r="223" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A223" s="58"/>
-      <c r="B223" s="59"/>
-      <c r="C223" s="59"/>
-      <c r="D223" s="59"/>
-      <c r="E223" s="59"/>
-      <c r="F223" s="59"/>
-      <c r="G223" s="64"/>
-      <c r="H223" s="64"/>
-      <c r="I223" s="64"/>
+      <c r="A223" s="59"/>
+      <c r="B223" s="60"/>
+      <c r="C223" s="60"/>
+      <c r="D223" s="60"/>
+      <c r="E223" s="60"/>
+      <c r="F223" s="60"/>
+      <c r="G223" s="65"/>
+      <c r="H223" s="65"/>
+      <c r="I223" s="65"/>
     </row>
     <row r="224" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A224" s="53"/>
-      <c r="B224" s="53"/>
+      <c r="A224" s="54"/>
+      <c r="B224" s="54"/>
       <c r="C224" s="35"/>
       <c r="D224" s="48"/>
       <c r="E224" s="48"/>
       <c r="F224" s="35"/>
-      <c r="G224" s="64"/>
-      <c r="H224" s="64"/>
-      <c r="I224" s="64"/>
+      <c r="G224" s="65"/>
+      <c r="H224" s="65"/>
+      <c r="I224" s="65"/>
     </row>
     <row r="225" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A225" s="53"/>
-      <c r="B225" s="53"/>
+      <c r="A225" s="54"/>
+      <c r="B225" s="54"/>
       <c r="C225" s="35"/>
       <c r="D225" s="48"/>
       <c r="E225" s="48"/>
       <c r="F225" s="35"/>
-      <c r="G225" s="64"/>
-      <c r="H225" s="64"/>
-      <c r="I225" s="64"/>
+      <c r="G225" s="65"/>
+      <c r="H225" s="65"/>
+      <c r="I225" s="65"/>
     </row>
     <row r="226" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A226" s="53"/>
-      <c r="B226" s="53"/>
+      <c r="A226" s="54"/>
+      <c r="B226" s="54"/>
       <c r="C226" s="35"/>
       <c r="D226" s="48"/>
       <c r="E226" s="48"/>
       <c r="F226" s="35"/>
-      <c r="G226" s="68"/>
-      <c r="H226" s="68"/>
-      <c r="I226" s="68"/>
+      <c r="G226" s="69"/>
+      <c r="H226" s="69"/>
+      <c r="I226" s="69"/>
     </row>
     <row r="227" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A227" s="53"/>
-      <c r="B227" s="53"/>
+      <c r="A227" s="54"/>
+      <c r="B227" s="54"/>
       <c r="C227" s="35"/>
       <c r="D227" s="48"/>
       <c r="E227" s="48"/>
       <c r="F227" s="35"/>
-      <c r="G227" s="64"/>
-      <c r="H227" s="64"/>
-      <c r="I227" s="64"/>
+      <c r="G227" s="65"/>
+      <c r="H227" s="65"/>
+      <c r="I227" s="65"/>
     </row>
     <row r="228" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A228" s="53"/>
-      <c r="B228" s="53"/>
+      <c r="A228" s="54"/>
+      <c r="B228" s="54"/>
       <c r="C228" s="35"/>
       <c r="D228" s="48"/>
       <c r="E228" s="48"/>
       <c r="F228" s="35"/>
-      <c r="G228" s="64"/>
-      <c r="H228" s="64"/>
-      <c r="I228" s="64"/>
+      <c r="G228" s="65"/>
+      <c r="H228" s="65"/>
+      <c r="I228" s="65"/>
     </row>
     <row r="229" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A229" s="53"/>
-      <c r="B229" s="53"/>
+      <c r="A229" s="54"/>
+      <c r="B229" s="54"/>
       <c r="C229" s="35"/>
       <c r="D229" s="48"/>
       <c r="E229" s="48"/>
       <c r="F229" s="35"/>
-      <c r="G229" s="64"/>
-      <c r="H229" s="64"/>
-      <c r="I229" s="64"/>
+      <c r="G229" s="65"/>
+      <c r="H229" s="65"/>
+      <c r="I229" s="65"/>
     </row>
     <row r="230" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A230" s="53"/>
-      <c r="B230" s="53"/>
+      <c r="A230" s="54"/>
+      <c r="B230" s="54"/>
       <c r="C230" s="35"/>
       <c r="D230" s="48"/>
       <c r="E230" s="48"/>
       <c r="F230" s="35"/>
-      <c r="G230" s="64"/>
-      <c r="H230" s="64"/>
-      <c r="I230" s="64"/>
+      <c r="G230" s="65"/>
+      <c r="H230" s="65"/>
+      <c r="I230" s="65"/>
     </row>
     <row r="231" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A231" s="53"/>
-      <c r="B231" s="53"/>
+      <c r="A231" s="54"/>
+      <c r="B231" s="54"/>
       <c r="C231" s="35"/>
       <c r="D231" s="48"/>
       <c r="E231" s="48"/>
       <c r="F231" s="35"/>
-      <c r="G231" s="64"/>
-      <c r="H231" s="64"/>
-      <c r="I231" s="64"/>
+      <c r="G231" s="65"/>
+      <c r="H231" s="65"/>
+      <c r="I231" s="65"/>
     </row>
     <row r="232" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A232" s="53"/>
-      <c r="B232" s="53"/>
+      <c r="A232" s="54"/>
+      <c r="B232" s="54"/>
       <c r="C232" s="35"/>
       <c r="D232" s="48"/>
       <c r="E232" s="48"/>
       <c r="F232" s="35"/>
-      <c r="G232" s="64"/>
-      <c r="H232" s="64"/>
-      <c r="I232" s="64"/>
+      <c r="G232" s="65"/>
+      <c r="H232" s="65"/>
+      <c r="I232" s="65"/>
     </row>
     <row r="233" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A233" s="53"/>
-      <c r="B233" s="53"/>
+      <c r="A233" s="54"/>
+      <c r="B233" s="54"/>
       <c r="C233" s="35"/>
       <c r="D233" s="48"/>
       <c r="E233" s="48"/>
       <c r="F233" s="35"/>
-      <c r="G233" s="64"/>
-      <c r="H233" s="64"/>
-      <c r="I233" s="64"/>
+      <c r="G233" s="65"/>
+      <c r="H233" s="65"/>
+      <c r="I233" s="65"/>
     </row>
     <row r="234" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A234" s="53"/>
-      <c r="B234" s="53"/>
+      <c r="A234" s="54"/>
+      <c r="B234" s="54"/>
       <c r="C234" s="35"/>
       <c r="D234" s="48"/>
       <c r="E234" s="48"/>
       <c r="F234" s="35"/>
-      <c r="G234" s="64"/>
-      <c r="H234" s="64"/>
-      <c r="I234" s="64"/>
+      <c r="G234" s="65"/>
+      <c r="H234" s="65"/>
+      <c r="I234" s="65"/>
     </row>
     <row r="235" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A235" s="53"/>
-      <c r="B235" s="53"/>
+      <c r="A235" s="54"/>
+      <c r="B235" s="54"/>
       <c r="C235" s="35"/>
       <c r="D235" s="48"/>
       <c r="E235" s="48"/>
       <c r="F235" s="35"/>
-      <c r="G235" s="64"/>
-      <c r="H235" s="64"/>
-      <c r="I235" s="64"/>
+      <c r="G235" s="65"/>
+      <c r="H235" s="65"/>
+      <c r="I235" s="65"/>
     </row>
     <row r="236" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A236" s="53"/>
-      <c r="B236" s="53"/>
+      <c r="A236" s="54"/>
+      <c r="B236" s="54"/>
       <c r="C236" s="35"/>
       <c r="D236" s="48"/>
       <c r="E236" s="48"/>
       <c r="F236" s="35"/>
-      <c r="G236" s="64"/>
-      <c r="H236" s="64"/>
-      <c r="I236" s="64"/>
+      <c r="G236" s="65"/>
+      <c r="H236" s="65"/>
+      <c r="I236" s="65"/>
     </row>
     <row r="237" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A237" s="53"/>
-      <c r="B237" s="53"/>
+      <c r="A237" s="54"/>
+      <c r="B237" s="54"/>
       <c r="C237" s="35"/>
       <c r="D237" s="48"/>
       <c r="E237" s="48"/>
       <c r="F237" s="35"/>
-      <c r="G237" s="64"/>
-      <c r="H237" s="64"/>
-      <c r="I237" s="64"/>
+      <c r="G237" s="65"/>
+      <c r="H237" s="65"/>
+      <c r="I237" s="65"/>
     </row>
     <row r="238" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A238" s="53"/>
-      <c r="B238" s="53"/>
+      <c r="A238" s="54"/>
+      <c r="B238" s="54"/>
       <c r="C238" s="35"/>
       <c r="D238" s="48"/>
       <c r="E238" s="48"/>
       <c r="F238" s="35"/>
-      <c r="G238" s="64"/>
-      <c r="H238" s="64"/>
-      <c r="I238" s="64"/>
+      <c r="G238" s="65"/>
+      <c r="H238" s="65"/>
+      <c r="I238" s="65"/>
     </row>
     <row r="239" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A239" s="53"/>
-      <c r="B239" s="53"/>
+      <c r="A239" s="54"/>
+      <c r="B239" s="54"/>
       <c r="C239" s="35"/>
       <c r="D239" s="48"/>
       <c r="E239" s="48"/>
       <c r="F239" s="35"/>
-      <c r="G239" s="64"/>
-      <c r="H239" s="64"/>
-      <c r="I239" s="64"/>
+      <c r="G239" s="65"/>
+      <c r="H239" s="65"/>
+      <c r="I239" s="65"/>
     </row>
     <row r="240" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A240" s="53"/>
-      <c r="B240" s="53"/>
+      <c r="A240" s="54"/>
+      <c r="B240" s="54"/>
       <c r="C240" s="35"/>
       <c r="D240" s="48"/>
       <c r="E240" s="48"/>
       <c r="F240" s="35"/>
-      <c r="G240" s="64"/>
-      <c r="H240" s="64"/>
-      <c r="I240" s="64"/>
+      <c r="G240" s="65"/>
+      <c r="H240" s="65"/>
+      <c r="I240" s="65"/>
     </row>
     <row r="241" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A241" s="53"/>
-      <c r="B241" s="53"/>
+      <c r="A241" s="54"/>
+      <c r="B241" s="54"/>
       <c r="C241" s="35"/>
       <c r="D241" s="48"/>
       <c r="E241" s="48"/>
       <c r="F241" s="35"/>
-      <c r="G241" s="64"/>
-      <c r="H241" s="64"/>
-      <c r="I241" s="64"/>
+      <c r="G241" s="65"/>
+      <c r="H241" s="65"/>
+      <c r="I241" s="65"/>
     </row>
     <row r="242" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A242" s="53"/>
-      <c r="B242" s="53"/>
+      <c r="A242" s="54"/>
+      <c r="B242" s="54"/>
       <c r="C242" s="35"/>
       <c r="D242" s="48"/>
       <c r="E242" s="48"/>
       <c r="F242" s="35"/>
-      <c r="G242" s="64"/>
-      <c r="H242" s="64"/>
-      <c r="I242" s="64"/>
+      <c r="G242" s="65"/>
+      <c r="H242" s="65"/>
+      <c r="I242" s="65"/>
     </row>
     <row r="243" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A243" s="53"/>
-      <c r="B243" s="53"/>
+      <c r="A243" s="54"/>
+      <c r="B243" s="54"/>
       <c r="C243" s="35"/>
       <c r="D243" s="48"/>
       <c r="E243" s="48"/>
       <c r="F243" s="35"/>
-      <c r="G243" s="64"/>
-      <c r="H243" s="64"/>
-      <c r="I243" s="64"/>
+      <c r="G243" s="65"/>
+      <c r="H243" s="65"/>
+      <c r="I243" s="65"/>
     </row>
     <row r="244" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A244" s="53"/>
-      <c r="B244" s="53"/>
+      <c r="A244" s="54"/>
+      <c r="B244" s="54"/>
       <c r="C244" s="35"/>
       <c r="D244" s="48"/>
       <c r="E244" s="48"/>
       <c r="F244" s="35"/>
-      <c r="G244" s="64"/>
-      <c r="H244" s="64"/>
-      <c r="I244" s="64"/>
+      <c r="G244" s="65"/>
+      <c r="H244" s="65"/>
+      <c r="I244" s="65"/>
     </row>
     <row r="245" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A245" s="53"/>
-      <c r="B245" s="53"/>
+      <c r="A245" s="54"/>
+      <c r="B245" s="54"/>
       <c r="C245" s="35"/>
       <c r="D245" s="48"/>
       <c r="E245" s="48"/>
       <c r="F245" s="35"/>
-      <c r="G245" s="64"/>
-      <c r="H245" s="64"/>
-      <c r="I245" s="64"/>
+      <c r="G245" s="65"/>
+      <c r="H245" s="65"/>
+      <c r="I245" s="65"/>
     </row>
     <row r="246" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A246" s="53"/>
-      <c r="B246" s="53"/>
+      <c r="A246" s="54"/>
+      <c r="B246" s="54"/>
       <c r="C246" s="35"/>
       <c r="D246" s="48"/>
       <c r="E246" s="48"/>
       <c r="F246" s="35"/>
-      <c r="G246" s="64"/>
-      <c r="H246" s="64"/>
-      <c r="I246" s="64"/>
+      <c r="G246" s="65"/>
+      <c r="H246" s="65"/>
+      <c r="I246" s="65"/>
     </row>
     <row r="247" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A247" s="53"/>
-      <c r="B247" s="53"/>
+      <c r="A247" s="54"/>
+      <c r="B247" s="54"/>
       <c r="C247" s="35"/>
       <c r="D247" s="48"/>
       <c r="E247" s="48"/>
       <c r="F247" s="35"/>
-      <c r="G247" s="64"/>
-      <c r="H247" s="64"/>
-      <c r="I247" s="64"/>
+      <c r="G247" s="65"/>
+      <c r="H247" s="65"/>
+      <c r="I247" s="65"/>
     </row>
     <row r="248" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A248" s="53"/>
-      <c r="B248" s="53"/>
+      <c r="A248" s="54"/>
+      <c r="B248" s="54"/>
       <c r="C248" s="35"/>
       <c r="D248" s="48"/>
       <c r="E248" s="48"/>
       <c r="F248" s="35"/>
-      <c r="G248" s="64"/>
-      <c r="H248" s="64"/>
-      <c r="I248" s="64"/>
+      <c r="G248" s="65"/>
+      <c r="H248" s="65"/>
+      <c r="I248" s="65"/>
     </row>
     <row r="249" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A249" s="53"/>
-      <c r="B249" s="53"/>
+      <c r="A249" s="54"/>
+      <c r="B249" s="54"/>
       <c r="C249" s="35"/>
       <c r="D249" s="48"/>
       <c r="E249" s="48"/>
       <c r="F249" s="35"/>
-      <c r="G249" s="64"/>
-      <c r="H249" s="64"/>
-      <c r="I249" s="64"/>
+      <c r="G249" s="65"/>
+      <c r="H249" s="65"/>
+      <c r="I249" s="65"/>
     </row>
     <row r="250" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
-      <c r="A250" s="53"/>
-      <c r="B250" s="53"/>
+      <c r="A250" s="54"/>
+      <c r="B250" s="54"/>
       <c r="C250" s="35"/>
       <c r="D250" s="48"/>
       <c r="E250" s="48"/>
       <c r="F250" s="35"/>
-      <c r="G250" s="64"/>
-      <c r="H250" s="64"/>
-      <c r="I250" s="64"/>
+      <c r="G250" s="65"/>
+      <c r="H250" s="65"/>
+      <c r="I250" s="65"/>
     </row>
     <row r="251" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
       <c r="A251" s="17"/>
@@ -4030,9 +3565,9 @@
       <c r="D251" s="16"/>
       <c r="E251" s="16"/>
       <c r="F251" s="19"/>
-      <c r="G251" s="69"/>
-      <c r="H251" s="69"/>
-      <c r="I251" s="69"/>
+      <c r="G251" s="70"/>
+      <c r="H251" s="70"/>
+      <c r="I251" s="70"/>
     </row>
     <row r="252" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
       <c r="A252" s="17"/>
@@ -4041,9 +3576,9 @@
       <c r="D252" s="16"/>
       <c r="E252" s="16"/>
       <c r="F252" s="19"/>
-      <c r="G252" s="69"/>
-      <c r="H252" s="69"/>
-      <c r="I252" s="69"/>
+      <c r="G252" s="70"/>
+      <c r="H252" s="70"/>
+      <c r="I252" s="70"/>
     </row>
     <row r="253" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
       <c r="A253" s="17"/>
@@ -4052,9 +3587,9 @@
       <c r="D253" s="16"/>
       <c r="E253" s="16"/>
       <c r="F253" s="19"/>
-      <c r="G253" s="69"/>
-      <c r="H253" s="69"/>
-      <c r="I253" s="69"/>
+      <c r="G253" s="70"/>
+      <c r="H253" s="70"/>
+      <c r="I253" s="70"/>
     </row>
     <row r="254" spans="1:10" customHeight="1" ht="39.75" s="6" customFormat="1">
       <c r="A254" s="17"/>
@@ -4063,9 +3598,9 @@
       <c r="D254" s="16"/>
       <c r="E254" s="16"/>
       <c r="F254" s="19"/>
-      <c r="G254" s="69"/>
-      <c r="H254" s="69"/>
-      <c r="I254" s="69"/>
+      <c r="G254" s="70"/>
+      <c r="H254" s="70"/>
+      <c r="I254" s="70"/>
     </row>
     <row r="255" spans="1:10" customHeight="1" ht="23.25" s="6" customFormat="1">
       <c r="A255" s="17"/>
@@ -10585,16 +10120,16 @@
         <v>43838</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="H1" s="12">
         <v>15183000</v>
@@ -10617,16 +10152,16 @@
         <v>43838</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="12">
         <v>1999000</v>
@@ -10649,16 +10184,16 @@
         <v>43838</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="G3" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="12">
         <v>1799000</v>
@@ -10681,16 +10216,16 @@
         <v>43860</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H4" s="12">
         <v>500000</v>
@@ -10713,16 +10248,16 @@
         <v>43838</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="G5" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H5" s="12">
         <v>15183000</v>
@@ -10745,16 +10280,16 @@
         <v>43838</v>
       </c>
       <c r="D6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="G6" s="15" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H6" s="12">
         <v>1999000</v>
@@ -10777,16 +10312,16 @@
         <v>43838</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="G7" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H7" s="12">
         <v>1798000</v>
@@ -10809,16 +10344,16 @@
         <v>43865</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H8" s="12">
         <v>296000</v>
@@ -10841,16 +10376,16 @@
         <v>43866</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H9" s="12">
         <v>688000</v>
@@ -10873,16 +10408,16 @@
         <v>43866</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H10" s="12">
         <v>100376</v>

</xml_diff>